<commit_message>
Add UMI fields to Excel report
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="257">
   <si>
     <t>af</t>
   </si>
@@ -755,6 +755,15 @@
   </si>
   <si>
     <t>transposition_transposase_source</t>
+  </si>
+  <si>
+    <t>umi_offset</t>
+  </si>
+  <si>
+    <t>umi_read</t>
+  </si>
+  <si>
+    <t>umi_size</t>
   </si>
   <si>
     <t>uniprot_accession_number</t>
@@ -1110,7 +1119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA228"/>
+  <dimension ref="A1:AA231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -4868,7 +4877,7 @@
       <c r="A222" t="s">
         <v>247</v>
       </c>
-      <c r="C222" t="s">
+      <c r="V222" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4876,73 +4885,7 @@
       <c r="A223" t="s">
         <v>248</v>
       </c>
-      <c r="B223" t="s">
-        <v>27</v>
-      </c>
-      <c r="C223" t="s">
-        <v>27</v>
-      </c>
-      <c r="D223" t="s">
-        <v>27</v>
-      </c>
-      <c r="E223" t="s">
-        <v>27</v>
-      </c>
-      <c r="F223" t="s">
-        <v>27</v>
-      </c>
-      <c r="G223" t="s">
-        <v>27</v>
-      </c>
-      <c r="H223" t="s">
-        <v>27</v>
-      </c>
-      <c r="I223" t="s">
-        <v>27</v>
-      </c>
-      <c r="K223" t="s">
-        <v>27</v>
-      </c>
-      <c r="L223" t="s">
-        <v>27</v>
-      </c>
-      <c r="M223" t="s">
-        <v>27</v>
-      </c>
-      <c r="N223" t="s">
-        <v>27</v>
-      </c>
-      <c r="O223" t="s">
-        <v>27</v>
-      </c>
-      <c r="P223" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q223" t="s">
-        <v>27</v>
-      </c>
-      <c r="R223" t="s">
-        <v>27</v>
-      </c>
-      <c r="S223" t="s">
-        <v>27</v>
-      </c>
-      <c r="U223" t="s">
-        <v>27</v>
-      </c>
       <c r="V223" t="s">
-        <v>27</v>
-      </c>
-      <c r="X223" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y223" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z223" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA223" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4950,39 +4893,129 @@
       <c r="A224" t="s">
         <v>249</v>
       </c>
-      <c r="T224" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="225" spans="1:20">
+      <c r="V224" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="225" spans="1:27">
       <c r="A225" t="s">
         <v>250</v>
       </c>
-      <c r="T225" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="226" spans="1:20">
+      <c r="C225" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="226" spans="1:27">
       <c r="A226" t="s">
         <v>251</v>
       </c>
-      <c r="T226" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="227" spans="1:20">
+      <c r="B226" t="s">
+        <v>27</v>
+      </c>
+      <c r="C226" t="s">
+        <v>27</v>
+      </c>
+      <c r="D226" t="s">
+        <v>27</v>
+      </c>
+      <c r="E226" t="s">
+        <v>27</v>
+      </c>
+      <c r="F226" t="s">
+        <v>27</v>
+      </c>
+      <c r="G226" t="s">
+        <v>27</v>
+      </c>
+      <c r="H226" t="s">
+        <v>27</v>
+      </c>
+      <c r="I226" t="s">
+        <v>27</v>
+      </c>
+      <c r="K226" t="s">
+        <v>27</v>
+      </c>
+      <c r="L226" t="s">
+        <v>27</v>
+      </c>
+      <c r="M226" t="s">
+        <v>27</v>
+      </c>
+      <c r="N226" t="s">
+        <v>27</v>
+      </c>
+      <c r="O226" t="s">
+        <v>27</v>
+      </c>
+      <c r="P226" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q226" t="s">
+        <v>27</v>
+      </c>
+      <c r="R226" t="s">
+        <v>27</v>
+      </c>
+      <c r="S226" t="s">
+        <v>27</v>
+      </c>
+      <c r="U226" t="s">
+        <v>27</v>
+      </c>
+      <c r="V226" t="s">
+        <v>27</v>
+      </c>
+      <c r="X226" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y226" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z226" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA226" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="227" spans="1:27">
       <c r="A227" t="s">
         <v>252</v>
       </c>
-      <c r="J227" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="228" spans="1:20">
+      <c r="T227" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="228" spans="1:27">
       <c r="A228" t="s">
         <v>253</v>
       </c>
-      <c r="J228" t="s">
+      <c r="T228" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="229" spans="1:27">
+      <c r="A229" t="s">
+        <v>254</v>
+      </c>
+      <c r="T229" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="230" spans="1:27">
+      <c r="A230" t="s">
+        <v>255</v>
+      </c>
+      <c r="J230" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="231" spans="1:27">
+      <c r="A231" t="s">
+        <v>256</v>
+      </c>
+      <c r="J231" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add descriptions as comments
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -13,6 +13,3007 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of x resolution distance between laser ablation shots.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>x resolution. Distance between laser ablation shots in the X-dimension.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of y resolution distance between laser ablation shots.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>y resolution. Distance between laser ablation shots in the Y-dimension.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Frequency unit of laser ablation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Frequency value of laser ablation (in Hz)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The acquisition_id refers to the directory containing the ROI images for a slide. Together, the acquisition_id and the roi_id indicate the slide-ROI represented in the image.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturers of an acquisition instrument may offer various versions (models) of that instrument with different features or sensitivities. Differences in features or sensitivities may be relevant to processing or interpretation of the data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An acquisition_instrument is the device that contains the signal detection hardware and signal processing software. Assays generate signals such as light of various intensities or color or signals representing molecular mass.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Institutional affiliation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for age measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The time elapsed since birth.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analytes are the target molecules being measured with the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative path to file with antibody information for this dataset.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anti-(target name) antibody. Not validated or used down-stream.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Area normalized ion dose unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of primary ions delivered to the sample per unit area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Each assay is placed into one of the following 4 general categories: generation of images of microscopic entities, identification &amp; quantitation of molecules by mass spectrometry, imaging mass spectrometry, and determination of nucleotide sequence.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The specific type of assay being executed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position(s) in the read at which the bead barcode starts</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Which read file contains the bead barcode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of the bead barcode in base pairs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ABO blood type or "serotype" refers to the presence/absence of the either/both A &amp; B blood antigens.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An individual's weight in kilograms divided by the square of the height in meters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to a protocols document answering the question: How was tissue stored and processed for cell/nuclei isolation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to a protocols document answering the question: How was tissue stored and processed for RNA isolation RNA_isolation_protocols_io_doi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RIN value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RNA amount per Tissue input amount. Valid values should be weight/weight (ng/mg).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RNA (ng) per Weight of Tissue (mg). Answer the question: How much RNA in ng was isolated? How much tissue in mg was initially used for isolating RNA? Calculate the yield by dividing total RNA isolated by amount of tissue used to isolate RNA from (ng/mg).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A number (no comma separators)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The circumstance or condition that caused death.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chemical composition of the background electrolyte that fills the separation capillary (e.g. "3% acetic acid").</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Treatment of surface of separation capillary. Capillary coating affects the absorption of analytes on capillary inner walls and regulates electroosmotic flow. Entries should indicate the charge of the coating and chemical composition (e.g. "Neutral; Polyacrylamide" or "Positive; Polyethyleneimine" or "Uncoated").</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Properties of the electroosmotic flow (EOF). Normal EOF is defined as flow towards the cathode, reversed EOF is defined as flow towards the anode, and suppressed EOF involves marginal to almost no flow (e.g. when a neutral coating is used).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model name of the instrument used for capillary zone electrophoresis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the instrument used for capillary zone electrophoresis. Capillary electrophoresis is used to separate complex biological mixtures prior to performing MS-based analyses. Separations are performed based the analytes migrate through an electrolyte solution in the presence of an electric field.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Method by which the separation capillary interfaces with mass spectrometer and enables electrospray ionization while completing the separation circuit. The two most prevalent commercial interfaces are sheathless and sheath-flow.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position(s) in the read at which the cell barcode starts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Which read file contains the cell barcode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of the cell barcode in base pairs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Structure of channel_id depends on assay type.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time interval on ice to the start of preservation protocol.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for GC column length</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GC column length</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model of the GC column used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units for GC column temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GC column temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the GC column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A51" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The concentration units of the antibody preparation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The concentration value of the antibody preparation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An antibody may be conjugated to a fluorescent tag or a metal tag for detection. Conjugated antibodies may be purchased from commercial providers.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The name of the entity conjugated to the antibody.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A55" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative path to file with ORCID IDs for contributors for this dataset.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition) or DIA (Data-independent acquisition).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A57" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative path to file or directory with instrument data. Downstream processing will depend on filename extension conventions.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Numerical data precision in bytes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Free-text description of this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solvent composition for conducting nanospray desorption electrospray ionization (nanoDESI) or desorption electrospray ionization (DESI).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A61" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The rate of flow of the solvent into a spray.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A62" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of the rate of solvent flow.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody solutions may be diluted according to the experimental protocol.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Was differential mobility spectrometry used in this assay?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A65" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of DNA input into library preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amount of DNA input into library preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A68" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Threshold for dual counting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A69" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time stamp indicating end of ablation for ROI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A70" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Start date and time of assay, typically a date-time stamped folder generated by the acquisition instrument. YYYY-MM-DD hh:mm, where YYYY is the year, MM is the month with leading 0s, and DD is the day with leading 0s, hh is the hour with leading zeros, mm are the minutes with leading zeros.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>How many cells are expected? This may be used in downstream pipelines to guide selection of cell barcodes or segmentation parameters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A72" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>First name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A73" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is the gDNA integrity good enough for WGS? This is usually checked through running a gel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A74" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies if guard column was used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patient's baseline physical condition prior to immediate event leading to organ/tissue acquisition. For example, if a relatively healthy patient suffers trauma, and as a result of reparative surgery, a tissue sample is collected, the subject will be deemed “relatively healthy”.   Likewise, a relatively healthy subject may have experienced trauma leading to brain death.  As a result of organ donation, a sample is collected.  In this scenario, the subject is deemed “relatively healthy.”</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A76" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for height measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A77" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The vertical measurement or distance from the base to the top of a subject or participant.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A78" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The units of increment z value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A79" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The distance between sequential optical sections.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A80" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies if internal standard was utilized and designates what standard was used. Leave blank if not applicable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A81" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not ion mobility spectrometry was performed and which technology was used. Technologies for measuring ion mobility: Traveling Wave Ion Mobility Spectrometry (TWIMS), Trapped Ion Mobility Spectrometry (TIMS), High Field Asymmetric waveform ion Mobility Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS, Structures for Lossless Ion Manipulations (SLIM).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A82" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies the ion source used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A83" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is this individual a contact for DOI purposes?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A84" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not a specific molecule(s) is/are targeted for detection/measurement by the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A85" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is this a sequencing replicate?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A86" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The Kidney Donor Profle Index (KDPI) is a numerical measure that combines ten donor factors, including clinical parameters and demographics, to summarize into a single number the quality of deceased donor kidneys relative to other recovered kidneys. The KDPI is derived by frst calculating the Kidney Donor Risk Index (KDRI) for a deceased donor. Kidneys from a donor with a KDPI of 90%, for example, have a KDRI (which indicates relative risk of graft failure) greater than 90% of recovered kidneys. The KDPI is simply a mapping of the KDRI from a relative risk scale to a cumulative percentage scale. The reference population used for this mapping is all deceased donors in the United States with a kidney recovered for the purpose of transplantation in the prior calendar year. Lower KDPI values are associated with increased donor quality and expected longevity. https://optn.transplant.hrsa.gov/media/1512/guide_to_calculating_interpreting_kdpi.pdf
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A87" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the samples were labeled (e.g. TMT), provide the name/ID of the label on this sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A88" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates whether samples were labeled prior to MS analysis (e.g., TMT)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A89" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Last name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A90" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model number/name of the LC Column - IF custom self-packed, pulled tip calillary is used enter "Pulled tip capilary"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A91" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPTIONAL: The manufacturer of the LC Column unless self-packed, pulled tip capilary is used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A92" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of flow rate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A93" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of flow rate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A94" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC gradient</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A95" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>units of LC column inner diameter (typically microns)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A96" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC column inner diameter (microns)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A97" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model number/name of the instrument used for LC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A98" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the instrument used for LC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A99" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>units for LC column length (typically cm)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A100" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC column length</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A101" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Composition of mobile phase A</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A102" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Composition of mobile phase B</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A103" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Details of the resin used for lc, including vendor, particle size, pore size</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A104" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>units for LC temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A105" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A106" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adapter sequence to be used for adapter trimming</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A107" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Average size in basepairs (bp) of sequencing library fragments estimated via gel electrophoresis or bioanalyzer/tapestation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A108" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit of library_concentration_value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A109" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The concentration value of the pooled library samples submitted for sequencing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A110" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Describes DNA library preparation kit. Modality of isolating gDNA, Fragmentation and generating sequencing libraries.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A111" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A link to the protocol document containing the library construction method (including version) that was used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A112" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>date and time of library creation. YYYY-MM-DD, where YYYY is the year, MM is the month with leading 0s, and DD is the day with leading 0s.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A113" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total ng of library after final pcr amplification step.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A114" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of final library yield</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A115" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of ng of library after final pcr amplification step. This is the concentration (ng/ul) * volume (ul)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A116" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An id for the library. The id may be text and/or numbers</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A117" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Whether the library was generated for single-end or paired end sequencing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A118" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of PCR cycles to amplify cDNA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A119" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of PCR cycles performed for library indexing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A120" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Reagent kit used for library preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A121" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The lot# is specific to the vendor. (eg: Abcam lot# GR3238979-1)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A122" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The MS1 resolving power defined as m/∆m where ∆m is the FWHM for a given peak with a specified m/z (m). (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A123" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of image width of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A124" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Image width value of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A125" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of image height of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A126" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Image height value of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A127" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mechanism of injury may be, for example: fall, impact (eg: auto accident), weapon (eg: firearm), etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A128" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A record of a patient's background regarding health and the occurrence of disease events of the individual.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A129" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Middle name or initial</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A130" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates whether the data were generated using MS, MS/MS or MS3.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A131" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The ion source type used for surface sampling.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A132" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The high value of the scanned mass range for MS1. (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A133" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The low value of the scanned mass range for MS1. (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A134" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The peak (m/z) used to calculate the resolving power.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A135" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name for display</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A136" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of antibodies</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A137" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of barcode probes targeting mRNAs (eg. 24,000 barcode probes = 24,000 mRNAs - 1 per mRNA of interest)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A138" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of barcode regions on each mRNA barcode probe (the paper describes mRNA probes with 4 barcoded regions)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A139" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of mass channels measured</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A140" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of cycles of 1. oligo application, 2. fluor application, 3. washes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A141" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the total number of acquisitions performed on microscope to collect autofluorescence/background or stained signal.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A142" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of pseudocolors that can be assigned to each fluorescent channel (the paper describes 20 pseudocolors per channel (x 3 channels -&gt; total = 60)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A143" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of readout probes that can be interrogated per channel per cycle (the paper describes 20 readout probes per channel (x 3 channels -&gt; total = 60))</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A144" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of sections</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A145" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the person responsible for executing the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A146" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Email address for the operator.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A147" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ORCID ID of contributor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A148" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Health status of the organ at the time of sample recovery.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A149" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io for the overall process.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A150" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Further details on organ level QC checks.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A151" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of solution that was used to perfuse the organ.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A152" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the principal investigator responsible for the data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A153" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Email address for the principal investigator.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A154" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pixel dwell time unit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A155" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resident time of primary ion beam on each pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A156" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Width unit of the pixel or voxel measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A157" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Width value of the pixel or voxel measurement (distinct from the image resolution_x_value).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A158" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length unit of the pixel or voxel measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A159" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length value of the pixel or voxel measurement (distinct from the image resolution_y_value).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A160" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The polarity of the mass analysis (positive or negative ion modes)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A161" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model number/name of the instrument used to prepare the sample for the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A162" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the instrument used to prepare the sample for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A163" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The matrix is a compound of crystallized molecules that acts like a buffer between the sample and the laser. It also helps ionize the sample, carrying it along the flight tube so it can be detected.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A164" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Common methods of depositing matrix for MALDI imaging include robotic spotting, electrospray deposition, and spray-coating with an airbrush.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A165" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Primary ion.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A166" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Primary ion current unit, typically nA or pA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A167" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Primary ion current value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A168" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of procedure to procure organ.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A169" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for analysis protocols.io for this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A170" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Software for analyzing and searching LC-MS/MS omics data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A171" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io referring to the protocol for this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A172" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Slide-seq captures RNA sequence data on spatially barcoded arrays of beads. Beads are fixed to a slide in a region shaped like a round puck. Each puck has a unique puck_id.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A173" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A grouping of humans based on shared physical characteristics or social/ethnic identity generally viewed as distinct.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A174" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of range_z_value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A175" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The total range of the z axis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A176" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io referring to the protocol for preparing reagents for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A177" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of measurement of the width of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A178" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The width of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A179" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of measurement of the height of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A180" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The height of a pixel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A181" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of incremental distance between image slices.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A182" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The distance at which two objects along the detection z-axis can be distinguished (resolved as 2 objects).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A183" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of cell/nuclei input to the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A184" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of RNA input amount to the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A185" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RNA input amount value to the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A186" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The kit used for the RNA sequencing assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A187" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A description of the region of interest (ROI) captured in the image.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A188" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Multiple images (1-n) are acquired from regions of interest (ROI1, ROI2, ROI3, etc) on a slide. The roi_id is a number from 1-n representing the ROI captured on a slide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A189" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The rr_id is a unique antibody identifier that comes from the Antibody Registry (https://antibodyregistry.org).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A190" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(No description for this field was supplied.)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A191" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a quality metric by visual inspection. This should answer the question: Are the nuclei intact and are the nuclei free of significant amounts of debris? This can be captured at a high level, “OK” or “not OK”.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A192" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of cell/nuclei yielded post dissociation and enrichment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A193" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The method by which specific cell populations are sorted or enriched.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A194" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The type of single cell entity derived from isolation protocol</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A195" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to a protocols document answering the question: How were single cells separated into a single-cell suspension?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A196" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A quality metric by visual inspection prior to cell lysis or defined by known parameters such as wells with several cells or no cells. This can be captured at a high level.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A197" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The method by which tissues are dissociated into single cells in suspension.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A198" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io referring to the protocol for preparing tissue sections for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A199" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This refers to the data type, which is a "float" for the IMC counts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A200" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Percent PhiX loaded to the run</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A201" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Slash-delimited list of the number of sequencing cycles for, for example, Read1, i7 index, i5 index, and Read2.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A202" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Q30 is the weighted average of all the reads (e.g. # bases UMI * q30 UMI + # bases R2 * q30 R2 + ...)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A203" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Reagent kit used for sequencing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A204" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Biological sex at birth: male or female or other.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A205" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of signal measured per channel (usually dual counts)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A206" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>External source (outside of HuBMAP) of the project, eg. HCA (The Human Cell Atlas Consortium).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A207" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not the analysis was performed in a spatially targeted manner. Spatial profiling experiments target specific tissue foci but do not necessarily generate images. Spatial imaging expriments collect data from a regular array (pixels) that can be visualized as heat maps of ion intensity at each location (molecular images). Leave blank if data are derived from bulk analysis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A208" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies the cell-type or functional tissue unit (FTU) that is targeted in the spatial profiling experiment. Leave blank if data are generated in imaging mode without a specific target structure.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A209" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not the analysis was performed in a spatialy targeted manner and the technique used for spatial sampling. For example, Laser-capture microdissection (LCM), Liquid Extraction Surface Analysis (LESA), Nanodroplet Processing in One pot for Trace Samples (nanoPOTS).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A210" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The temperature of the medium during the preservation process.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A211" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>For example, RIN: 8.7.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A212" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Distance unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A213" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If surgical sample, how far from the tumor was the sample obtained from. Typically a number of centimeters. Leave blank if not applicable or unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A214" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chemical stains (dyes) applied to histology samples to highlight important features of the tissue as well as to enhance the tissue contrast.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A215" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time stamp indicating start of ablation for ROI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A216" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The number of optical sections in z axis range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A217" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>HuBMAP Display ID of the assayed tissue.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A218" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of cell/nuclei input to the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A219" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If Tn5 came from a kit, provide the catalog number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A220" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Modality of capturing accessible chromatin molecules.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A221" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The source of the Tn5 transposase and transposon used for capturing accessible chromatin.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A222" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position in the read at which the umi barcode starts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A223" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Which read file(s) contains the UMI (unique molecular identifier) barcode.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A224" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of the umi barcode in base pairs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A225" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The uniprot_accession_number is a unique identifier for proteins in the UniProt database (https://www.uniprot.org).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A226" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Version of the schema to use when validating this metadata.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A227" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identify the vital state of the donor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A228" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A229" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time interval between cessation of blood flow and cooling to 4C.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A230" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for weight measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A231" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A measurement that describes the vertical force exerted by a mass of the patient as a result of gravity.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="257">
   <si>
@@ -791,13 +3792,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5021,5 +8028,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mccalluc/excel add descriptions (#1021)
* add descriptions as comments

* md typo

* enumerate_from_1

* whitespace
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -13,6 +13,3007 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of x resolution distance between laser ablation shots.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>x resolution. Distance between laser ablation shots in the X-dimension.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of y resolution distance between laser ablation shots.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>y resolution. Distance between laser ablation shots in the Y-dimension.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Frequency unit of laser ablation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Frequency value of laser ablation (in Hz)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The acquisition_id refers to the directory containing the ROI images for a slide. Together, the acquisition_id and the roi_id indicate the slide-ROI represented in the image.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturers of an acquisition instrument may offer various versions (models) of that instrument with different features or sensitivities. Differences in features or sensitivities may be relevant to processing or interpretation of the data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An acquisition_instrument is the device that contains the signal detection hardware and signal processing software. Assays generate signals such as light of various intensities or color or signals representing molecular mass.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Institutional affiliation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for age measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The time elapsed since birth.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analytes are the target molecules being measured with the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative path to file with antibody information for this dataset.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anti-(target name) antibody. Not validated or used down-stream.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Area normalized ion dose unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of primary ions delivered to the sample per unit area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Each assay is placed into one of the following 4 general categories: generation of images of microscopic entities, identification &amp; quantitation of molecules by mass spectrometry, imaging mass spectrometry, and determination of nucleotide sequence.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The specific type of assay being executed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position(s) in the read at which the bead barcode starts</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Which read file contains the bead barcode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of the bead barcode in base pairs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ABO blood type or "serotype" refers to the presence/absence of the either/both A &amp; B blood antigens.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An individual's weight in kilograms divided by the square of the height in meters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to a protocols document answering the question: How was tissue stored and processed for cell/nuclei isolation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to a protocols document answering the question: How was tissue stored and processed for RNA isolation RNA_isolation_protocols_io_doi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RIN value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RNA amount per Tissue input amount. Valid values should be weight/weight (ng/mg).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RNA (ng) per Weight of Tissue (mg). Answer the question: How much RNA in ng was isolated? How much tissue in mg was initially used for isolating RNA? Calculate the yield by dividing total RNA isolated by amount of tissue used to isolate RNA from (ng/mg).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A number (no comma separators)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The circumstance or condition that caused death.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chemical composition of the background electrolyte that fills the separation capillary (e.g. "3% acetic acid").</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Treatment of surface of separation capillary. Capillary coating affects the absorption of analytes on capillary inner walls and regulates electroosmotic flow. Entries should indicate the charge of the coating and chemical composition (e.g. "Neutral; Polyacrylamide" or "Positive; Polyethyleneimine" or "Uncoated").</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Properties of the electroosmotic flow (EOF). Normal EOF is defined as flow towards the cathode, reversed EOF is defined as flow towards the anode, and suppressed EOF involves marginal to almost no flow (e.g. when a neutral coating is used).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model name of the instrument used for capillary zone electrophoresis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the instrument used for capillary zone electrophoresis. Capillary electrophoresis is used to separate complex biological mixtures prior to performing MS-based analyses. Separations are performed based the analytes migrate through an electrolyte solution in the presence of an electric field.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Method by which the separation capillary interfaces with mass spectrometer and enables electrospray ionization while completing the separation circuit. The two most prevalent commercial interfaces are sheathless and sheath-flow.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position(s) in the read at which the cell barcode starts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Which read file contains the cell barcode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of the cell barcode in base pairs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Structure of channel_id depends on assay type.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time interval on ice to the start of preservation protocol.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for GC column length</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GC column length</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model of the GC column used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units for GC column temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GC column temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the GC column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A51" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The concentration units of the antibody preparation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The concentration value of the antibody preparation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An antibody may be conjugated to a fluorescent tag or a metal tag for detection. Conjugated antibodies may be purchased from commercial providers.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The name of the entity conjugated to the antibody.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A55" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative path to file with ORCID IDs for contributors for this dataset.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition) or DIA (Data-independent acquisition).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A57" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative path to file or directory with instrument data. Downstream processing will depend on filename extension conventions.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Numerical data precision in bytes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Free-text description of this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Solvent composition for conducting nanospray desorption electrospray ionization (nanoDESI) or desorption electrospray ionization (DESI).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A61" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The rate of flow of the solvent into a spray.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A62" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of the rate of solvent flow.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody solutions may be diluted according to the experimental protocol.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Was differential mobility spectrometry used in this assay?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A65" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of DNA input into library preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amount of DNA input into library preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A68" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Threshold for dual counting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A69" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time stamp indicating end of ablation for ROI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A70" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Start date and time of assay, typically a date-time stamped folder generated by the acquisition instrument. YYYY-MM-DD hh:mm, where YYYY is the year, MM is the month with leading 0s, and DD is the day with leading 0s, hh is the hour with leading zeros, mm are the minutes with leading zeros.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>How many cells are expected? This may be used in downstream pipelines to guide selection of cell barcodes or segmentation parameters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A72" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>First name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A73" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is the gDNA integrity good enough for WGS? This is usually checked through running a gel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A74" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies if guard column was used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patient's baseline physical condition prior to immediate event leading to organ/tissue acquisition. For example, if a relatively healthy patient suffers trauma, and as a result of reparative surgery, a tissue sample is collected, the subject will be deemed “relatively healthy”.   Likewise, a relatively healthy subject may have experienced trauma leading to brain death.  As a result of organ donation, a sample is collected.  In this scenario, the subject is deemed “relatively healthy.”</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A76" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for height measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A77" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The vertical measurement or distance from the base to the top of a subject or participant.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A78" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The units of increment z value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A79" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The distance between sequential optical sections.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A80" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies if internal standard was utilized and designates what standard was used. Leave blank if not applicable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A81" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not ion mobility spectrometry was performed and which technology was used. Technologies for measuring ion mobility: Traveling Wave Ion Mobility Spectrometry (TWIMS), Trapped Ion Mobility Spectrometry (TIMS), High Field Asymmetric waveform ion Mobility Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS, Structures for Lossless Ion Manipulations (SLIM).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A82" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies the ion source used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A83" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is this individual a contact for DOI purposes?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A84" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not a specific molecule(s) is/are targeted for detection/measurement by the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A85" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is this a sequencing replicate?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A86" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The Kidney Donor Profle Index (KDPI) is a numerical measure that combines ten donor factors, including clinical parameters and demographics, to summarize into a single number the quality of deceased donor kidneys relative to other recovered kidneys. The KDPI is derived by frst calculating the Kidney Donor Risk Index (KDRI) for a deceased donor. Kidneys from a donor with a KDPI of 90%, for example, have a KDRI (which indicates relative risk of graft failure) greater than 90% of recovered kidneys. The KDPI is simply a mapping of the KDRI from a relative risk scale to a cumulative percentage scale. The reference population used for this mapping is all deceased donors in the United States with a kidney recovered for the purpose of transplantation in the prior calendar year. Lower KDPI values are associated with increased donor quality and expected longevity. https://optn.transplant.hrsa.gov/media/1512/guide_to_calculating_interpreting_kdpi.pdf
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A87" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the samples were labeled (e.g. TMT), provide the name/ID of the label on this sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A88" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates whether samples were labeled prior to MS analysis (e.g., TMT)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A89" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Last name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A90" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model number/name of the LC Column - IF custom self-packed, pulled tip calillary is used enter "Pulled tip capilary"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A91" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPTIONAL: The manufacturer of the LC Column unless self-packed, pulled tip capilary is used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A92" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of flow rate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A93" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of flow rate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A94" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC gradient</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A95" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>units of LC column inner diameter (typically microns)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A96" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC column inner diameter (microns)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A97" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model number/name of the instrument used for LC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A98" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the instrument used for LC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A99" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>units for LC column length (typically cm)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A100" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC column length</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A101" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Composition of mobile phase A</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A102" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Composition of mobile phase B</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A103" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Details of the resin used for lc, including vendor, particle size, pore size</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A104" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>units for LC temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A105" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LC temperature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A106" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adapter sequence to be used for adapter trimming</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A107" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Average size in basepairs (bp) of sequencing library fragments estimated via gel electrophoresis or bioanalyzer/tapestation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A108" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit of library_concentration_value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A109" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The concentration value of the pooled library samples submitted for sequencing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A110" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Describes DNA library preparation kit. Modality of isolating gDNA, Fragmentation and generating sequencing libraries.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A111" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A link to the protocol document containing the library construction method (including version) that was used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A112" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>date and time of library creation. YYYY-MM-DD, where YYYY is the year, MM is the month with leading 0s, and DD is the day with leading 0s.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A113" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total ng of library after final pcr amplification step.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A114" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of final library yield</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A115" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of ng of library after final pcr amplification step. This is the concentration (ng/ul) * volume (ul)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A116" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An id for the library. The id may be text and/or numbers</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A117" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Whether the library was generated for single-end or paired end sequencing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A118" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of PCR cycles to amplify cDNA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A119" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of PCR cycles performed for library indexing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A120" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Reagent kit used for library preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A121" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The lot# is specific to the vendor. (eg: Abcam lot# GR3238979-1)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A122" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The MS1 resolving power defined as m/∆m where ∆m is the FWHM for a given peak with a specified m/z (m). (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A123" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of image width of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A124" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Image width value of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A125" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of image height of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A126" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Image height value of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A127" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mechanism of injury may be, for example: fall, impact (eg: auto accident), weapon (eg: firearm), etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A128" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A record of a patient's background regarding health and the occurrence of disease events of the individual.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A129" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Middle name or initial</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A130" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates whether the data were generated using MS, MS/MS or MS3.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A131" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The ion source type used for surface sampling.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A132" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The high value of the scanned mass range for MS1. (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A133" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The low value of the scanned mass range for MS1. (unitless)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A134" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The peak (m/z) used to calculate the resolving power.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A135" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name for display</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A136" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of antibodies</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A137" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of barcode probes targeting mRNAs (eg. 24,000 barcode probes = 24,000 mRNAs - 1 per mRNA of interest)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A138" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of barcode regions on each mRNA barcode probe (the paper describes mRNA probes with 4 barcoded regions)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A139" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of mass channels measured</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A140" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of cycles of 1. oligo application, 2. fluor application, 3. washes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A141" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the total number of acquisitions performed on microscope to collect autofluorescence/background or stained signal.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A142" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of pseudocolors that can be assigned to each fluorescent channel (the paper describes 20 pseudocolors per channel (x 3 channels -&gt; total = 60)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A143" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of readout probes that can be interrogated per channel per cycle (the paper describes 20 readout probes per channel (x 3 channels -&gt; total = 60))</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A144" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of sections</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A145" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the person responsible for executing the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A146" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Email address for the operator.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A147" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ORCID ID of contributor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A148" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Health status of the organ at the time of sample recovery.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A149" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io for the overall process.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A150" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Further details on organ level QC checks.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A151" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of solution that was used to perfuse the organ.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A152" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the principal investigator responsible for the data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A153" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Email address for the principal investigator.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A154" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pixel dwell time unit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A155" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resident time of primary ion beam on each pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A156" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Width unit of the pixel or voxel measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A157" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Width value of the pixel or voxel measurement (distinct from the image resolution_x_value).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A158" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length unit of the pixel or voxel measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A159" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length value of the pixel or voxel measurement (distinct from the image resolution_y_value).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A160" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The polarity of the mass analysis (positive or negative ion modes)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A161" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The model number/name of the instrument used to prepare the sample for the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A162" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The manufacturer of the instrument used to prepare the sample for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A163" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The matrix is a compound of crystallized molecules that acts like a buffer between the sample and the laser. It also helps ionize the sample, carrying it along the flight tube so it can be detected.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A164" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Common methods of depositing matrix for MALDI imaging include robotic spotting, electrospray deposition, and spray-coating with an airbrush.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A165" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Primary ion.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A166" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Primary ion current unit, typically nA or pA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A167" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Primary ion current value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A168" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of procedure to procure organ.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A169" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for analysis protocols.io for this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A170" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Software for analyzing and searching LC-MS/MS omics data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A171" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io referring to the protocol for this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A172" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Slide-seq captures RNA sequence data on spatially barcoded arrays of beads. Beads are fixed to a slide in a region shaped like a round puck. Each puck has a unique puck_id.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A173" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A grouping of humans based on shared physical characteristics or social/ethnic identity generally viewed as distinct.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A174" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of range_z_value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A175" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The total range of the z axis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A176" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io referring to the protocol for preparing reagents for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A177" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of measurement of the width of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A178" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The width of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A179" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of measurement of the height of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A180" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The height of a pixel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A181" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of incremental distance between image slices.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A182" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The distance at which two objects along the detection z-axis can be distinguished (resolved as 2 objects).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A183" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of cell/nuclei input to the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A184" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of RNA input amount to the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A185" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RNA input amount value to the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A186" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The kit used for the RNA sequencing assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A187" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A description of the region of interest (ROI) captured in the image.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A188" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Multiple images (1-n) are acquired from regions of interest (ROI1, ROI2, ROI3, etc) on a slide. The roi_id is a number from 1-n representing the ROI captured on a slide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A189" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The rr_id is a unique antibody identifier that comes from the Antibody Registry (https://antibodyregistry.org).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A190" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(No description for this field was supplied.)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A191" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a quality metric by visual inspection. This should answer the question: Are the nuclei intact and are the nuclei free of significant amounts of debris? This can be captured at a high level, “OK” or “not OK”.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A192" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of cell/nuclei yielded post dissociation and enrichment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A193" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The method by which specific cell populations are sorted or enriched.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A194" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The type of single cell entity derived from isolation protocol</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A195" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to a protocols document answering the question: How were single cells separated into a single-cell suspension?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A196" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A quality metric by visual inspection prior to cell lysis or defined by known parameters such as wells with several cells or no cells. This can be captured at a high level.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A197" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The method by which tissues are dissociated into single cells in suspension.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A198" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DOI for protocols.io referring to the protocol for preparing tissue sections for the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A199" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This refers to the data type, which is a "float" for the IMC counts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A200" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Percent PhiX loaded to the run</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A201" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Slash-delimited list of the number of sequencing cycles for, for example, Read1, i7 index, i5 index, and Read2.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A202" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Q30 is the weighted average of all the reads (e.g. # bases UMI * q30 UMI + # bases R2 * q30 R2 + ...)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A203" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Reagent kit used for sequencing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A204" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Biological sex at birth: male or female or other.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A205" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of signal measured per channel (usually dual counts)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A206" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>External source (outside of HuBMAP) of the project, eg. HCA (The Human Cell Atlas Consortium).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A207" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not the analysis was performed in a spatially targeted manner. Spatial profiling experiments target specific tissue foci but do not necessarily generate images. Spatial imaging expriments collect data from a regular array (pixels) that can be visualized as heat maps of ion intensity at each location (molecular images). Leave blank if data are derived from bulk analysis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A208" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies the cell-type or functional tissue unit (FTU) that is targeted in the spatial profiling experiment. Leave blank if data are generated in imaging mode without a specific target structure.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A209" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not the analysis was performed in a spatialy targeted manner and the technique used for spatial sampling. For example, Laser-capture microdissection (LCM), Liquid Extraction Surface Analysis (LESA), Nanodroplet Processing in One pot for Trace Samples (nanoPOTS).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A210" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The temperature of the medium during the preservation process.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A211" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>For example, RIN: 8.7.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A212" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Distance unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A213" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If surgical sample, how far from the tumor was the sample obtained from. Typically a number of centimeters. Leave blank if not applicable or unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A214" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chemical stains (dyes) applied to histology samples to highlight important features of the tissue as well as to enhance the tissue contrast.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A215" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time stamp indicating start of ablation for ROI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A216" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The number of optical sections in z axis range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A217" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>HuBMAP Display ID of the assayed tissue.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A218" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of cell/nuclei input to the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A219" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If Tn5 came from a kit, provide the catalog number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A220" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Modality of capturing accessible chromatin molecules.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A221" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The source of the Tn5 transposase and transposon used for capturing accessible chromatin.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A222" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Position in the read at which the umi barcode starts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A223" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Which read file(s) contains the UMI (unique molecular identifier) barcode.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A224" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of the umi barcode in base pairs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A225" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The uniprot_accession_number is a unique identifier for proteins in the UniProt database (https://www.uniprot.org).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A226" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Version of the schema to use when validating this metadata.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A227" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identify the vital state of the donor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A228" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A229" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time interval between cessation of blood flow and cooling to 4C.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A230" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit for weight measurement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A231" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A measurement that describes the vertical force exerted by a mass of the patient as a result of gravity.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="257">
   <si>
@@ -791,13 +3792,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5021,5 +8028,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add missing pathology_distance_unit (#1072)
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2018,11 +2018,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Distance unit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A156" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>If surgical sample, how far from the pathology was the sample obtained. Typically a number of centimeters. Leave blank if not applicable or unknown.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A156" authorId="0">
+    <comment ref="A157" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2035,7 +2048,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A157" authorId="0">
+    <comment ref="A158" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2048,7 +2061,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A158" authorId="0">
+    <comment ref="A159" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2061,7 +2074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A159" authorId="0">
+    <comment ref="A160" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2074,7 +2087,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A160" authorId="0">
+    <comment ref="A161" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2087,7 +2100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A161" authorId="0">
+    <comment ref="A162" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2100,7 +2113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A162" authorId="0">
+    <comment ref="A163" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2113,7 +2126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A163" authorId="0">
+    <comment ref="A164" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2126,7 +2139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A164" authorId="0">
+    <comment ref="A165" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2139,7 +2152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A165" authorId="0">
+    <comment ref="A166" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2152,7 +2165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A166" authorId="0">
+    <comment ref="A167" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2165,7 +2178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A167" authorId="0">
+    <comment ref="A168" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2178,7 +2191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A168" authorId="0">
+    <comment ref="A169" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2191,7 +2204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A169" authorId="0">
+    <comment ref="A170" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2204,7 +2217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A170" authorId="0">
+    <comment ref="A171" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2217,7 +2230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A171" authorId="0">
+    <comment ref="A172" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2230,7 +2243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A172" authorId="0">
+    <comment ref="A173" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2243,7 +2256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A173" authorId="0">
+    <comment ref="A174" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2256,7 +2269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A174" authorId="0">
+    <comment ref="A175" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2269,7 +2282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A175" authorId="0">
+    <comment ref="A176" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2282,7 +2295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A176" authorId="0">
+    <comment ref="A177" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2295,7 +2308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A177" authorId="0">
+    <comment ref="A178" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2308,7 +2321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A178" authorId="0">
+    <comment ref="A179" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2321,7 +2334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A179" authorId="0">
+    <comment ref="A180" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2334,7 +2347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A180" authorId="0">
+    <comment ref="A181" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2347,7 +2360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A181" authorId="0">
+    <comment ref="A182" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2360,7 +2373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A182" authorId="0">
+    <comment ref="A183" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2373,7 +2386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A183" authorId="0">
+    <comment ref="A184" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2386,7 +2399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A184" authorId="0">
+    <comment ref="A185" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2399,7 +2412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A185" authorId="0">
+    <comment ref="A186" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2412,7 +2425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A186" authorId="0">
+    <comment ref="A187" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2425,7 +2438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A187" authorId="0">
+    <comment ref="A188" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2438,7 +2451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A188" authorId="0">
+    <comment ref="A189" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2451,7 +2464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A189" authorId="0">
+    <comment ref="A190" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2464,7 +2477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A190" authorId="0">
+    <comment ref="A191" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2477,7 +2490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A191" authorId="0">
+    <comment ref="A192" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2490,7 +2503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A192" authorId="0">
+    <comment ref="A193" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2503,7 +2516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A193" authorId="0">
+    <comment ref="A194" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2516,7 +2529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A194" authorId="0">
+    <comment ref="A195" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2529,7 +2542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A195" authorId="0">
+    <comment ref="A196" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2542,7 +2555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A196" authorId="0">
+    <comment ref="A197" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2555,7 +2568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A197" authorId="0">
+    <comment ref="A198" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2568,7 +2581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A198" authorId="0">
+    <comment ref="A199" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2581,7 +2594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A199" authorId="0">
+    <comment ref="A200" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2594,7 +2607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A200" authorId="0">
+    <comment ref="A201" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2607,7 +2620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A201" authorId="0">
+    <comment ref="A202" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2620,7 +2633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A202" authorId="0">
+    <comment ref="A203" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2633,7 +2646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A203" authorId="0">
+    <comment ref="A204" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2646,7 +2659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A204" authorId="0">
+    <comment ref="A205" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2659,7 +2672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A205" authorId="0">
+    <comment ref="A206" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2672,7 +2685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A206" authorId="0">
+    <comment ref="A207" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2685,7 +2698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A207" authorId="0">
+    <comment ref="A208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2698,7 +2711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A208" authorId="0">
+    <comment ref="A209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2711,7 +2724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A209" authorId="0">
+    <comment ref="A210" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2724,7 +2737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A210" authorId="0">
+    <comment ref="A211" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2737,7 +2750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A211" authorId="0">
+    <comment ref="A212" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2750,7 +2763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A212" authorId="0">
+    <comment ref="A213" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2763,7 +2776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A213" authorId="0">
+    <comment ref="A214" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2776,7 +2789,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A214" authorId="0">
+    <comment ref="A215" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2789,7 +2802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A215" authorId="0">
+    <comment ref="A216" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2802,7 +2815,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A216" authorId="0">
+    <comment ref="A217" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2815,7 +2828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A217" authorId="0">
+    <comment ref="A218" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2828,7 +2841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A218" authorId="0">
+    <comment ref="A219" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2841,7 +2854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A219" authorId="0">
+    <comment ref="A220" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2854,7 +2867,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A220" authorId="0">
+    <comment ref="A221" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2867,7 +2880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A221" authorId="0">
+    <comment ref="A222" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2880,7 +2893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A222" authorId="0">
+    <comment ref="A223" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2893,7 +2906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A223" authorId="0">
+    <comment ref="A224" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2906,7 +2919,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A224" authorId="0">
+    <comment ref="A225" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2919,7 +2932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A225" authorId="0">
+    <comment ref="A226" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2932,7 +2945,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A226" authorId="0">
+    <comment ref="A227" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2945,7 +2958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A227" authorId="0">
+    <comment ref="A228" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2958,7 +2971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A228" authorId="0">
+    <comment ref="A229" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2971,7 +2984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A229" authorId="0">
+    <comment ref="A230" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2984,7 +2997,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A230" authorId="0">
+    <comment ref="A231" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2997,7 +3010,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A231" authorId="0">
+    <comment ref="A232" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3010,7 +3023,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A232" authorId="0">
+    <comment ref="A233" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3023,7 +3036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A233" authorId="0">
+    <comment ref="A234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3036,7 +3049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A234" authorId="0">
+    <comment ref="A235" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3049,7 +3062,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A235" authorId="0">
+    <comment ref="A236" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3062,7 +3075,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A236" authorId="0">
+    <comment ref="A237" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3075,7 +3088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A237" authorId="0">
+    <comment ref="A238" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3088,7 +3101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A238" authorId="0">
+    <comment ref="A239" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3101,7 +3114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A239" authorId="0">
+    <comment ref="A240" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3114,7 +3127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A240" authorId="0">
+    <comment ref="A241" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3127,7 +3140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A241" authorId="0">
+    <comment ref="A242" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3140,7 +3153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A242" authorId="0">
+    <comment ref="A243" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3153,7 +3166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A243" authorId="0">
+    <comment ref="A244" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3166,7 +3179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A244" authorId="0">
+    <comment ref="A245" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3179,7 +3192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A245" authorId="0">
+    <comment ref="A246" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3192,7 +3205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A246" authorId="0">
+    <comment ref="A247" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3205,7 +3218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A247" authorId="0">
+    <comment ref="A248" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3218,7 +3231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A248" authorId="0">
+    <comment ref="A249" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3231,7 +3244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A249" authorId="0">
+    <comment ref="A250" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3244,7 +3257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A250" authorId="0">
+    <comment ref="A251" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3257,7 +3270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A251" authorId="0">
+    <comment ref="A252" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3275,7 +3288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="281">
   <si>
     <t>af</t>
   </si>
@@ -3824,6 +3837,9 @@
   </si>
   <si>
     <t>pathologist_report</t>
+  </si>
+  <si>
+    <t>pathology_distance_unit</t>
   </si>
   <si>
     <t>pathology_distance_value</t>
@@ -4455,7 +4471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD251"/>
+  <dimension ref="A1:AD252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -7019,7 +7035,7 @@
       <c r="A156" t="s">
         <v>184</v>
       </c>
-      <c r="T156" t="s">
+      <c r="U156" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7027,70 +7043,7 @@
       <c r="A157" t="s">
         <v>185</v>
       </c>
-      <c r="B157" t="s">
-        <v>30</v>
-      </c>
-      <c r="D157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E157" t="s">
-        <v>30</v>
-      </c>
-      <c r="F157" t="s">
-        <v>30</v>
-      </c>
-      <c r="G157" t="s">
-        <v>30</v>
-      </c>
-      <c r="H157" t="s">
-        <v>30</v>
-      </c>
-      <c r="K157" t="s">
-        <v>30</v>
-      </c>
-      <c r="L157" t="s">
-        <v>30</v>
-      </c>
-      <c r="M157" t="s">
-        <v>30</v>
-      </c>
-      <c r="N157" t="s">
-        <v>30</v>
-      </c>
-      <c r="O157" t="s">
-        <v>30</v>
-      </c>
-      <c r="P157" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q157" t="s">
-        <v>30</v>
-      </c>
-      <c r="R157" t="s">
-        <v>30</v>
-      </c>
-      <c r="S157" t="s">
-        <v>30</v>
-      </c>
-      <c r="X157" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y157" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z157" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA157" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB157" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC157" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD157" t="s">
+      <c r="T157" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7169,7 +7122,70 @@
       <c r="A159" t="s">
         <v>187</v>
       </c>
+      <c r="B159" t="s">
+        <v>30</v>
+      </c>
+      <c r="D159" t="s">
+        <v>30</v>
+      </c>
+      <c r="E159" t="s">
+        <v>30</v>
+      </c>
+      <c r="F159" t="s">
+        <v>30</v>
+      </c>
+      <c r="G159" t="s">
+        <v>30</v>
+      </c>
+      <c r="H159" t="s">
+        <v>30</v>
+      </c>
+      <c r="K159" t="s">
+        <v>30</v>
+      </c>
+      <c r="L159" t="s">
+        <v>30</v>
+      </c>
+      <c r="M159" t="s">
+        <v>30</v>
+      </c>
+      <c r="N159" t="s">
+        <v>30</v>
+      </c>
+      <c r="O159" t="s">
+        <v>30</v>
+      </c>
+      <c r="P159" t="s">
+        <v>30</v>
+      </c>
       <c r="Q159" t="s">
+        <v>30</v>
+      </c>
+      <c r="R159" t="s">
+        <v>30</v>
+      </c>
+      <c r="S159" t="s">
+        <v>30</v>
+      </c>
+      <c r="X159" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y159" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z159" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA159" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB159" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC159" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD159" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7217,19 +7233,7 @@
       <c r="A165" t="s">
         <v>193</v>
       </c>
-      <c r="G165" t="s">
-        <v>30</v>
-      </c>
-      <c r="K165" t="s">
-        <v>30</v>
-      </c>
-      <c r="N165" t="s">
-        <v>30</v>
-      </c>
-      <c r="O165" t="s">
-        <v>30</v>
-      </c>
-      <c r="S165" t="s">
+      <c r="Q165" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7237,22 +7241,19 @@
       <c r="A166" t="s">
         <v>194</v>
       </c>
-      <c r="H166" t="s">
-        <v>30</v>
-      </c>
-      <c r="L166" t="s">
-        <v>30</v>
-      </c>
-      <c r="M166" t="s">
+      <c r="G166" t="s">
+        <v>30</v>
+      </c>
+      <c r="K166" t="s">
         <v>30</v>
       </c>
       <c r="N166" t="s">
         <v>30</v>
       </c>
-      <c r="Q166" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA166" t="s">
+      <c r="O166" t="s">
+        <v>30</v>
+      </c>
+      <c r="S166" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7283,7 +7284,22 @@
       <c r="A168" t="s">
         <v>196</v>
       </c>
+      <c r="H168" t="s">
+        <v>30</v>
+      </c>
+      <c r="L168" t="s">
+        <v>30</v>
+      </c>
+      <c r="M168" t="s">
+        <v>30</v>
+      </c>
       <c r="N168" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q168" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA168" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7291,13 +7307,7 @@
       <c r="A169" t="s">
         <v>197</v>
       </c>
-      <c r="U169" t="s">
-        <v>30</v>
-      </c>
-      <c r="V169" t="s">
-        <v>30</v>
-      </c>
-      <c r="W169" t="s">
+      <c r="N169" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7319,7 +7329,13 @@
       <c r="A171" t="s">
         <v>199</v>
       </c>
-      <c r="N171" t="s">
+      <c r="U171" t="s">
+        <v>30</v>
+      </c>
+      <c r="V171" t="s">
+        <v>30</v>
+      </c>
+      <c r="W171" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7327,7 +7343,7 @@
       <c r="A172" t="s">
         <v>200</v>
       </c>
-      <c r="Q172" t="s">
+      <c r="N172" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7351,7 +7367,7 @@
       <c r="A175" t="s">
         <v>203</v>
       </c>
-      <c r="T175" t="s">
+      <c r="Q175" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7359,19 +7375,7 @@
       <c r="A176" t="s">
         <v>204</v>
       </c>
-      <c r="F176" t="s">
-        <v>30</v>
-      </c>
-      <c r="G176" t="s">
-        <v>30</v>
-      </c>
-      <c r="N176" t="s">
-        <v>30</v>
-      </c>
-      <c r="O176" t="s">
-        <v>30</v>
-      </c>
-      <c r="S176" t="s">
+      <c r="T176" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7379,13 +7383,19 @@
       <c r="A177" t="s">
         <v>205</v>
       </c>
+      <c r="F177" t="s">
+        <v>30</v>
+      </c>
       <c r="G177" t="s">
         <v>30</v>
       </c>
-      <c r="K177" t="s">
+      <c r="N177" t="s">
         <v>30</v>
       </c>
       <c r="O177" t="s">
+        <v>30</v>
+      </c>
+      <c r="S177" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7393,13 +7403,13 @@
       <c r="A178" t="s">
         <v>206</v>
       </c>
-      <c r="U178" t="s">
-        <v>30</v>
-      </c>
-      <c r="V178" t="s">
-        <v>30</v>
-      </c>
-      <c r="W178" t="s">
+      <c r="G178" t="s">
+        <v>30</v>
+      </c>
+      <c r="K178" t="s">
+        <v>30</v>
+      </c>
+      <c r="O178" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7421,70 +7431,13 @@
       <c r="A180" t="s">
         <v>208</v>
       </c>
-      <c r="B180" t="s">
-        <v>30</v>
-      </c>
-      <c r="D180" t="s">
-        <v>30</v>
-      </c>
-      <c r="E180" t="s">
-        <v>30</v>
-      </c>
-      <c r="F180" t="s">
-        <v>30</v>
-      </c>
-      <c r="G180" t="s">
-        <v>30</v>
-      </c>
-      <c r="H180" t="s">
-        <v>30</v>
-      </c>
-      <c r="K180" t="s">
-        <v>30</v>
-      </c>
-      <c r="L180" t="s">
-        <v>30</v>
-      </c>
-      <c r="M180" t="s">
-        <v>30</v>
-      </c>
-      <c r="N180" t="s">
-        <v>30</v>
-      </c>
-      <c r="O180" t="s">
-        <v>30</v>
-      </c>
-      <c r="P180" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q180" t="s">
-        <v>30</v>
-      </c>
-      <c r="R180" t="s">
-        <v>30</v>
-      </c>
-      <c r="S180" t="s">
-        <v>30</v>
-      </c>
-      <c r="X180" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y180" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z180" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA180" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB180" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC180" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD180" t="s">
+      <c r="U180" t="s">
+        <v>30</v>
+      </c>
+      <c r="V180" t="s">
+        <v>30</v>
+      </c>
+      <c r="W180" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7492,7 +7445,70 @@
       <c r="A181" t="s">
         <v>209</v>
       </c>
+      <c r="B181" t="s">
+        <v>30</v>
+      </c>
+      <c r="D181" t="s">
+        <v>30</v>
+      </c>
+      <c r="E181" t="s">
+        <v>30</v>
+      </c>
+      <c r="F181" t="s">
+        <v>30</v>
+      </c>
+      <c r="G181" t="s">
+        <v>30</v>
+      </c>
+      <c r="H181" t="s">
+        <v>30</v>
+      </c>
+      <c r="K181" t="s">
+        <v>30</v>
+      </c>
+      <c r="L181" t="s">
+        <v>30</v>
+      </c>
+      <c r="M181" t="s">
+        <v>30</v>
+      </c>
+      <c r="N181" t="s">
+        <v>30</v>
+      </c>
+      <c r="O181" t="s">
+        <v>30</v>
+      </c>
+      <c r="P181" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>30</v>
+      </c>
+      <c r="R181" t="s">
+        <v>30</v>
+      </c>
+      <c r="S181" t="s">
+        <v>30</v>
+      </c>
+      <c r="X181" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y181" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z181" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA181" t="s">
+        <v>30</v>
+      </c>
       <c r="AB181" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC181" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD181" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7500,13 +7516,7 @@
       <c r="A182" t="s">
         <v>210</v>
       </c>
-      <c r="U182" t="s">
-        <v>30</v>
-      </c>
-      <c r="V182" t="s">
-        <v>30</v>
-      </c>
-      <c r="W182" t="s">
+      <c r="AB182" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7514,7 +7524,13 @@
       <c r="A183" t="s">
         <v>211</v>
       </c>
-      <c r="J183" t="s">
+      <c r="U183" t="s">
+        <v>30</v>
+      </c>
+      <c r="V183" t="s">
+        <v>30</v>
+      </c>
+      <c r="W183" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7522,7 +7538,7 @@
       <c r="A184" t="s">
         <v>212</v>
       </c>
-      <c r="P184" t="s">
+      <c r="J184" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7538,22 +7554,7 @@
       <c r="A186" t="s">
         <v>214</v>
       </c>
-      <c r="H186" t="s">
-        <v>30</v>
-      </c>
-      <c r="L186" t="s">
-        <v>30</v>
-      </c>
-      <c r="M186" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q186" t="s">
-        <v>30</v>
-      </c>
-      <c r="R186" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA186" t="s">
+      <c r="P186" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7561,28 +7562,13 @@
       <c r="A187" t="s">
         <v>215</v>
       </c>
-      <c r="B187" t="s">
-        <v>30</v>
-      </c>
-      <c r="F187" t="s">
-        <v>30</v>
-      </c>
-      <c r="G187" t="s">
-        <v>30</v>
-      </c>
       <c r="H187" t="s">
         <v>30</v>
       </c>
-      <c r="K187" t="s">
-        <v>30</v>
-      </c>
-      <c r="N187" t="s">
-        <v>30</v>
-      </c>
-      <c r="O187" t="s">
-        <v>30</v>
-      </c>
-      <c r="P187" t="s">
+      <c r="L187" t="s">
+        <v>30</v>
+      </c>
+      <c r="M187" t="s">
         <v>30</v>
       </c>
       <c r="Q187" t="s">
@@ -7591,13 +7577,7 @@
       <c r="R187" t="s">
         <v>30</v>
       </c>
-      <c r="S187" t="s">
-        <v>30</v>
-      </c>
       <c r="AA187" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC187" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7740,10 +7720,34 @@
       <c r="B191" t="s">
         <v>30</v>
       </c>
+      <c r="F191" t="s">
+        <v>30</v>
+      </c>
+      <c r="G191" t="s">
+        <v>30</v>
+      </c>
       <c r="H191" t="s">
         <v>30</v>
       </c>
+      <c r="K191" t="s">
+        <v>30</v>
+      </c>
+      <c r="N191" t="s">
+        <v>30</v>
+      </c>
+      <c r="O191" t="s">
+        <v>30</v>
+      </c>
       <c r="P191" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q191" t="s">
+        <v>30</v>
+      </c>
+      <c r="R191" t="s">
+        <v>30</v>
+      </c>
+      <c r="S191" t="s">
         <v>30</v>
       </c>
       <c r="AA191" t="s">
@@ -7773,26 +7777,38 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:28">
+    <row r="193" spans="1:29">
       <c r="A193" t="s">
         <v>221</v>
       </c>
-      <c r="Y193" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z193" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="194" spans="1:28">
+      <c r="B193" t="s">
+        <v>30</v>
+      </c>
+      <c r="H193" t="s">
+        <v>30</v>
+      </c>
+      <c r="P193" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA193" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC193" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="194" spans="1:29">
       <c r="A194" t="s">
         <v>222</v>
       </c>
-      <c r="E194" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="195" spans="1:28">
+      <c r="Y194" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z194" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="195" spans="1:29">
       <c r="A195" t="s">
         <v>223</v>
       </c>
@@ -7800,38 +7816,32 @@
         <v>30</v>
       </c>
     </row>
-    <row r="196" spans="1:28">
+    <row r="196" spans="1:29">
       <c r="A196" t="s">
         <v>224</v>
       </c>
       <c r="E196" t="s">
         <v>30</v>
       </c>
-      <c r="Y196" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z196" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB196" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="197" spans="1:28">
+    </row>
+    <row r="197" spans="1:29">
       <c r="A197" t="s">
         <v>225</v>
       </c>
-      <c r="L197" t="s">
-        <v>30</v>
-      </c>
-      <c r="M197" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q197" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="198" spans="1:28">
+      <c r="E197" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y197" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z197" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB197" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="198" spans="1:29">
       <c r="A198" t="s">
         <v>226</v>
       </c>
@@ -7845,54 +7855,54 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="1:28">
+    <row r="199" spans="1:29">
       <c r="A199" t="s">
         <v>227</v>
       </c>
-      <c r="C199" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="200" spans="1:28">
+      <c r="L199" t="s">
+        <v>30</v>
+      </c>
+      <c r="M199" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q199" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="200" spans="1:29">
       <c r="A200" t="s">
         <v>228</v>
       </c>
-      <c r="T200" t="s">
-        <v>30</v>
-      </c>
-      <c r="U200" t="s">
-        <v>30</v>
-      </c>
-      <c r="V200" t="s">
-        <v>30</v>
-      </c>
-      <c r="W200" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="201" spans="1:28">
+      <c r="C200" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="201" spans="1:29">
       <c r="A201" t="s">
         <v>229</v>
       </c>
-      <c r="D201" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="202" spans="1:28">
+      <c r="T201" t="s">
+        <v>30</v>
+      </c>
+      <c r="U201" t="s">
+        <v>30</v>
+      </c>
+      <c r="V201" t="s">
+        <v>30</v>
+      </c>
+      <c r="W201" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="202" spans="1:29">
       <c r="A202" t="s">
         <v>230</v>
       </c>
-      <c r="X202" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y202" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z202" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="203" spans="1:28">
+      <c r="D202" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="203" spans="1:29">
       <c r="A203" t="s">
         <v>231</v>
       </c>
@@ -7906,7 +7916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="204" spans="1:28">
+    <row r="204" spans="1:29">
       <c r="A204" t="s">
         <v>232</v>
       </c>
@@ -7920,7 +7930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="205" spans="1:28">
+    <row r="205" spans="1:29">
       <c r="A205" t="s">
         <v>233</v>
       </c>
@@ -7934,7 +7944,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="1:28">
+    <row r="206" spans="1:29">
       <c r="A206" t="s">
         <v>234</v>
       </c>
@@ -7948,7 +7958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:28">
+    <row r="207" spans="1:29">
       <c r="A207" t="s">
         <v>235</v>
       </c>
@@ -7962,14 +7972,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:28">
+    <row r="208" spans="1:29">
       <c r="A208" t="s">
         <v>236</v>
       </c>
-      <c r="V208" t="s">
-        <v>30</v>
-      </c>
-      <c r="W208" t="s">
+      <c r="X208" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y208" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z208" t="s">
         <v>30</v>
       </c>
     </row>
@@ -7977,37 +7990,10 @@
       <c r="A209" t="s">
         <v>237</v>
       </c>
-      <c r="G209" t="s">
-        <v>30</v>
-      </c>
-      <c r="H209" t="s">
-        <v>30</v>
-      </c>
-      <c r="K209" t="s">
-        <v>30</v>
-      </c>
-      <c r="L209" t="s">
-        <v>30</v>
-      </c>
-      <c r="M209" t="s">
-        <v>30</v>
-      </c>
-      <c r="N209" t="s">
-        <v>30</v>
-      </c>
-      <c r="O209" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q209" t="s">
-        <v>30</v>
-      </c>
-      <c r="R209" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA209" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC209" t="s">
+      <c r="V209" t="s">
+        <v>30</v>
+      </c>
+      <c r="W209" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8015,10 +8001,37 @@
       <c r="A210" t="s">
         <v>238</v>
       </c>
-      <c r="V210" t="s">
-        <v>30</v>
-      </c>
-      <c r="W210" t="s">
+      <c r="G210" t="s">
+        <v>30</v>
+      </c>
+      <c r="H210" t="s">
+        <v>30</v>
+      </c>
+      <c r="K210" t="s">
+        <v>30</v>
+      </c>
+      <c r="L210" t="s">
+        <v>30</v>
+      </c>
+      <c r="M210" t="s">
+        <v>30</v>
+      </c>
+      <c r="N210" t="s">
+        <v>30</v>
+      </c>
+      <c r="O210" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q210" t="s">
+        <v>30</v>
+      </c>
+      <c r="R210" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA210" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC210" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8037,13 +8050,10 @@
       <c r="A212" t="s">
         <v>240</v>
       </c>
-      <c r="L212" t="s">
-        <v>30</v>
-      </c>
-      <c r="M212" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q212" t="s">
+      <c r="V212" t="s">
+        <v>30</v>
+      </c>
+      <c r="W212" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8051,25 +8061,13 @@
       <c r="A213" t="s">
         <v>241</v>
       </c>
-      <c r="D213" t="s">
-        <v>30</v>
-      </c>
-      <c r="E213" t="s">
-        <v>30</v>
-      </c>
-      <c r="X213" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y213" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z213" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB213" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD213" t="s">
+      <c r="L213" t="s">
+        <v>30</v>
+      </c>
+      <c r="M213" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q213" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8155,7 +8153,25 @@
       <c r="A217" t="s">
         <v>245</v>
       </c>
-      <c r="J217" t="s">
+      <c r="D217" t="s">
+        <v>30</v>
+      </c>
+      <c r="E217" t="s">
+        <v>30</v>
+      </c>
+      <c r="X217" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y217" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z217" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB217" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD217" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8163,13 +8179,7 @@
       <c r="A218" t="s">
         <v>246</v>
       </c>
-      <c r="L218" t="s">
-        <v>30</v>
-      </c>
-      <c r="M218" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q218" t="s">
+      <c r="J218" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8177,7 +8187,13 @@
       <c r="A219" t="s">
         <v>247</v>
       </c>
-      <c r="Z219" t="s">
+      <c r="L219" t="s">
+        <v>30</v>
+      </c>
+      <c r="M219" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q219" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8185,13 +8201,7 @@
       <c r="A220" t="s">
         <v>248</v>
       </c>
-      <c r="U220" t="s">
-        <v>30</v>
-      </c>
-      <c r="V220" t="s">
-        <v>30</v>
-      </c>
-      <c r="W220" t="s">
+      <c r="Z220" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8213,13 +8223,13 @@
       <c r="A222" t="s">
         <v>250</v>
       </c>
-      <c r="G222" t="s">
-        <v>30</v>
-      </c>
-      <c r="K222" t="s">
-        <v>30</v>
-      </c>
-      <c r="O222" t="s">
+      <c r="U222" t="s">
+        <v>30</v>
+      </c>
+      <c r="V222" t="s">
+        <v>30</v>
+      </c>
+      <c r="W222" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8255,7 +8265,13 @@
       <c r="A225" t="s">
         <v>253</v>
       </c>
-      <c r="T225" t="s">
+      <c r="G225" t="s">
+        <v>30</v>
+      </c>
+      <c r="K225" t="s">
+        <v>30</v>
+      </c>
+      <c r="O225" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8287,7 +8303,7 @@
       <c r="A229" t="s">
         <v>257</v>
       </c>
-      <c r="AC229" t="s">
+      <c r="T229" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8295,10 +8311,7 @@
       <c r="A230" t="s">
         <v>258</v>
       </c>
-      <c r="L230" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q230" t="s">
+      <c r="AC230" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8306,7 +8319,10 @@
       <c r="A231" t="s">
         <v>259</v>
       </c>
-      <c r="P231" t="s">
+      <c r="L231" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q231" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8314,13 +8330,7 @@
       <c r="A232" t="s">
         <v>260</v>
       </c>
-      <c r="U232" t="s">
-        <v>30</v>
-      </c>
-      <c r="V232" t="s">
-        <v>30</v>
-      </c>
-      <c r="W232" t="s">
+      <c r="P232" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8342,70 +8352,13 @@
       <c r="A234" t="s">
         <v>262</v>
       </c>
-      <c r="B234" t="s">
-        <v>30</v>
-      </c>
-      <c r="D234" t="s">
-        <v>30</v>
-      </c>
-      <c r="E234" t="s">
-        <v>30</v>
-      </c>
-      <c r="F234" t="s">
-        <v>30</v>
-      </c>
-      <c r="G234" t="s">
-        <v>30</v>
-      </c>
-      <c r="H234" t="s">
-        <v>30</v>
-      </c>
-      <c r="K234" t="s">
-        <v>30</v>
-      </c>
-      <c r="L234" t="s">
-        <v>30</v>
-      </c>
-      <c r="M234" t="s">
-        <v>30</v>
-      </c>
-      <c r="N234" t="s">
-        <v>30</v>
-      </c>
-      <c r="O234" t="s">
-        <v>30</v>
-      </c>
-      <c r="P234" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q234" t="s">
-        <v>30</v>
-      </c>
-      <c r="R234" t="s">
-        <v>30</v>
-      </c>
-      <c r="S234" t="s">
-        <v>30</v>
-      </c>
-      <c r="X234" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y234" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z234" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA234" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB234" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC234" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD234" t="s">
+      <c r="U234" t="s">
+        <v>30</v>
+      </c>
+      <c r="V234" t="s">
+        <v>30</v>
+      </c>
+      <c r="W234" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8413,7 +8366,70 @@
       <c r="A235" t="s">
         <v>263</v>
       </c>
+      <c r="B235" t="s">
+        <v>30</v>
+      </c>
+      <c r="D235" t="s">
+        <v>30</v>
+      </c>
+      <c r="E235" t="s">
+        <v>30</v>
+      </c>
+      <c r="F235" t="s">
+        <v>30</v>
+      </c>
+      <c r="G235" t="s">
+        <v>30</v>
+      </c>
+      <c r="H235" t="s">
+        <v>30</v>
+      </c>
+      <c r="K235" t="s">
+        <v>30</v>
+      </c>
+      <c r="L235" t="s">
+        <v>30</v>
+      </c>
+      <c r="M235" t="s">
+        <v>30</v>
+      </c>
+      <c r="N235" t="s">
+        <v>30</v>
+      </c>
+      <c r="O235" t="s">
+        <v>30</v>
+      </c>
+      <c r="P235" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q235" t="s">
+        <v>30</v>
+      </c>
+      <c r="R235" t="s">
+        <v>30</v>
+      </c>
+      <c r="S235" t="s">
+        <v>30</v>
+      </c>
       <c r="X235" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y235" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z235" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA235" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB235" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC235" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD235" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8421,9 +8437,6 @@
       <c r="A236" t="s">
         <v>264</v>
       </c>
-      <c r="D236" t="s">
-        <v>30</v>
-      </c>
       <c r="X236" t="s">
         <v>30</v>
       </c>
@@ -8454,13 +8467,10 @@
       <c r="A239" t="s">
         <v>267</v>
       </c>
-      <c r="U239" t="s">
-        <v>30</v>
-      </c>
-      <c r="V239" t="s">
-        <v>30</v>
-      </c>
-      <c r="W239" t="s">
+      <c r="D239" t="s">
+        <v>30</v>
+      </c>
+      <c r="X239" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8468,7 +8478,13 @@
       <c r="A240" t="s">
         <v>268</v>
       </c>
-      <c r="Y240" t="s">
+      <c r="U240" t="s">
+        <v>30</v>
+      </c>
+      <c r="V240" t="s">
+        <v>30</v>
+      </c>
+      <c r="W240" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8492,7 +8508,7 @@
       <c r="A243" t="s">
         <v>271</v>
       </c>
-      <c r="C243" t="s">
+      <c r="Y243" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8500,82 +8516,7 @@
       <c r="A244" t="s">
         <v>272</v>
       </c>
-      <c r="B244" t="s">
-        <v>30</v>
-      </c>
       <c r="C244" t="s">
-        <v>30</v>
-      </c>
-      <c r="D244" t="s">
-        <v>30</v>
-      </c>
-      <c r="E244" t="s">
-        <v>30</v>
-      </c>
-      <c r="F244" t="s">
-        <v>30</v>
-      </c>
-      <c r="G244" t="s">
-        <v>30</v>
-      </c>
-      <c r="H244" t="s">
-        <v>30</v>
-      </c>
-      <c r="I244" t="s">
-        <v>30</v>
-      </c>
-      <c r="K244" t="s">
-        <v>30</v>
-      </c>
-      <c r="L244" t="s">
-        <v>30</v>
-      </c>
-      <c r="M244" t="s">
-        <v>30</v>
-      </c>
-      <c r="N244" t="s">
-        <v>30</v>
-      </c>
-      <c r="O244" t="s">
-        <v>30</v>
-      </c>
-      <c r="P244" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q244" t="s">
-        <v>30</v>
-      </c>
-      <c r="R244" t="s">
-        <v>30</v>
-      </c>
-      <c r="S244" t="s">
-        <v>30</v>
-      </c>
-      <c r="U244" t="s">
-        <v>30</v>
-      </c>
-      <c r="V244" t="s">
-        <v>30</v>
-      </c>
-      <c r="W244" t="s">
-        <v>30</v>
-      </c>
-      <c r="X244" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y244" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA244" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB244" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC244" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD244" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8583,7 +8524,82 @@
       <c r="A245" t="s">
         <v>273</v>
       </c>
-      <c r="T245" t="s">
+      <c r="B245" t="s">
+        <v>30</v>
+      </c>
+      <c r="C245" t="s">
+        <v>30</v>
+      </c>
+      <c r="D245" t="s">
+        <v>30</v>
+      </c>
+      <c r="E245" t="s">
+        <v>30</v>
+      </c>
+      <c r="F245" t="s">
+        <v>30</v>
+      </c>
+      <c r="G245" t="s">
+        <v>30</v>
+      </c>
+      <c r="H245" t="s">
+        <v>30</v>
+      </c>
+      <c r="I245" t="s">
+        <v>30</v>
+      </c>
+      <c r="K245" t="s">
+        <v>30</v>
+      </c>
+      <c r="L245" t="s">
+        <v>30</v>
+      </c>
+      <c r="M245" t="s">
+        <v>30</v>
+      </c>
+      <c r="N245" t="s">
+        <v>30</v>
+      </c>
+      <c r="O245" t="s">
+        <v>30</v>
+      </c>
+      <c r="P245" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q245" t="s">
+        <v>30</v>
+      </c>
+      <c r="R245" t="s">
+        <v>30</v>
+      </c>
+      <c r="S245" t="s">
+        <v>30</v>
+      </c>
+      <c r="U245" t="s">
+        <v>30</v>
+      </c>
+      <c r="V245" t="s">
+        <v>30</v>
+      </c>
+      <c r="W245" t="s">
+        <v>30</v>
+      </c>
+      <c r="X245" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y245" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA245" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB245" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC245" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD245" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8591,7 +8607,7 @@
       <c r="A246" t="s">
         <v>274</v>
       </c>
-      <c r="U246" t="s">
+      <c r="T246" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8607,7 +8623,7 @@
       <c r="A248" t="s">
         <v>276</v>
       </c>
-      <c r="T248" t="s">
+      <c r="U248" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8623,10 +8639,7 @@
       <c r="A250" t="s">
         <v>278</v>
       </c>
-      <c r="J250" t="s">
-        <v>30</v>
-      </c>
-      <c r="U250" t="s">
+      <c r="T250" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8638,6 +8651,17 @@
         <v>30</v>
       </c>
       <c r="U251" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="252" spans="1:30">
+      <c r="A252" t="s">
+        <v>280</v>
+      </c>
+      <c r="J252" t="s">
+        <v>30</v>
+      </c>
+      <c r="U252" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Few more fields, and regen
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -808,7 +808,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of the current used to acquire microCT images. Example: amp</t>
+          <t>The unit of the current used to acquire microCT images. Example: mA</t>
         </r>
       </text>
     </comment>
@@ -3240,7 +3240,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>TODO</t>
+          <t>The format in which each single imaging file will be exported. (Example: DICOM, tiff, avi, etc.)</t>
         </r>
       </text>
     </comment>
@@ -3500,7 +3500,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The number of sections used for analyzing microCT images</t>
+          <t>The number of sections used for analyzing microCT or OCT images</t>
         </r>
       </text>
     </comment>
@@ -3656,7 +3656,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of the voltage used to acquire microCT images. Example: volt</t>
+          <t>The unit of the voltage used to acquire microCT images. Example: V</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Update to comply with CI tasks
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3487,11 +3487,63 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Was the cell/nuclei population enriched?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A269" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the suspension was enriched, then this is the target of the enrichment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A270" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The type of single cell entity derived from isolation protocol.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A271" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of cell/nuclei yielded post dissociation and enrichment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A272" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A269" authorId="0">
+    <comment ref="A273" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3504,7 +3556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A270" authorId="0">
+    <comment ref="A274" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3517,7 +3569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A271" authorId="0">
+    <comment ref="A275" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3530,7 +3582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A272" authorId="0">
+    <comment ref="A276" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3543,7 +3595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A273" authorId="0">
+    <comment ref="A277" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3556,7 +3608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A274" authorId="0">
+    <comment ref="A278" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3569,7 +3621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A275" authorId="0">
+    <comment ref="A279" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3582,7 +3634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A276" authorId="0">
+    <comment ref="A280" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3595,7 +3647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A277" authorId="0">
+    <comment ref="A281" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3608,7 +3660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A278" authorId="0">
+    <comment ref="A282" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3621,7 +3673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A279" authorId="0">
+    <comment ref="A283" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3634,7 +3686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A280" authorId="0">
+    <comment ref="A284" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3647,7 +3699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A281" authorId="0">
+    <comment ref="A285" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3660,7 +3712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A282" authorId="0">
+    <comment ref="A286" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3673,7 +3725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A283" authorId="0">
+    <comment ref="A287" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3686,7 +3738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A284" authorId="0">
+    <comment ref="A288" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3699,7 +3751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A285" authorId="0">
+    <comment ref="A289" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3712,7 +3764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A286" authorId="0">
+    <comment ref="A290" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3725,7 +3777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A287" authorId="0">
+    <comment ref="A291" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3738,7 +3790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A288" authorId="0">
+    <comment ref="A292" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3751,7 +3803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A289" authorId="0">
+    <comment ref="A293" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3764,7 +3816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A290" authorId="0">
+    <comment ref="A294" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3777,7 +3829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A291" authorId="0">
+    <comment ref="A295" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3795,7 +3847,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="329">
   <si>
     <t>af</t>
   </si>
@@ -4698,6 +4750,18 @@
   </si>
   <si>
     <t>storage_temperature</t>
+  </si>
+  <si>
+    <t>suspension_enriched</t>
+  </si>
+  <si>
+    <t>suspension_enriched_target</t>
+  </si>
+  <si>
+    <t>suspension_entity</t>
+  </si>
+  <si>
+    <t>suspension_entity_number</t>
   </si>
   <si>
     <t>tissue_id</t>
@@ -5110,7 +5174,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI291"/>
+  <dimension ref="A1:AI295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -5649,9 +5713,6 @@
       <c r="Z21" t="s">
         <v>35</v>
       </c>
-      <c r="AA21" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="22" spans="1:35">
       <c r="A22" t="s">
@@ -5660,9 +5721,6 @@
       <c r="Z22" t="s">
         <v>35</v>
       </c>
-      <c r="AA22" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="23" spans="1:35">
       <c r="A23" t="s">
@@ -9303,9 +9361,6 @@
       <c r="Z237" t="s">
         <v>35</v>
       </c>
-      <c r="AA237" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="238" spans="1:34">
       <c r="A238" t="s">
@@ -9352,9 +9407,6 @@
       <c r="Z239" t="s">
         <v>35</v>
       </c>
-      <c r="AA239" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="240" spans="1:34">
       <c r="A240" t="s">
@@ -9363,9 +9415,6 @@
       <c r="Z240" t="s">
         <v>35</v>
       </c>
-      <c r="AA240" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="241" spans="1:35">
       <c r="A241" t="s">
@@ -9728,85 +9777,7 @@
       <c r="A268" t="s">
         <v>301</v>
       </c>
-      <c r="B268" t="s">
-        <v>35</v>
-      </c>
-      <c r="D268" t="s">
-        <v>35</v>
-      </c>
-      <c r="E268" t="s">
-        <v>35</v>
-      </c>
-      <c r="F268" t="s">
-        <v>35</v>
-      </c>
-      <c r="G268" t="s">
-        <v>35</v>
-      </c>
-      <c r="H268" t="s">
-        <v>35</v>
-      </c>
-      <c r="I268" t="s">
-        <v>35</v>
-      </c>
-      <c r="L268" t="s">
-        <v>35</v>
-      </c>
-      <c r="M268" t="s">
-        <v>35</v>
-      </c>
-      <c r="N268" t="s">
-        <v>35</v>
-      </c>
-      <c r="O268" t="s">
-        <v>35</v>
-      </c>
-      <c r="P268" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q268" t="s">
-        <v>35</v>
-      </c>
-      <c r="R268" t="s">
-        <v>35</v>
-      </c>
-      <c r="S268" t="s">
-        <v>35</v>
-      </c>
-      <c r="T268" t="s">
-        <v>35</v>
-      </c>
-      <c r="U268" t="s">
-        <v>35</v>
-      </c>
-      <c r="V268" t="s">
-        <v>35</v>
-      </c>
-      <c r="W268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH268" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI268" t="s">
+      <c r="AA268" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9814,10 +9785,7 @@
       <c r="A269" t="s">
         <v>302</v>
       </c>
-      <c r="S269" t="s">
-        <v>35</v>
-      </c>
-      <c r="W269" t="s">
+      <c r="AA269" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9825,7 +9793,7 @@
       <c r="A270" t="s">
         <v>303</v>
       </c>
-      <c r="AB270" t="s">
+      <c r="AA270" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9833,10 +9801,7 @@
       <c r="A271" t="s">
         <v>304</v>
       </c>
-      <c r="E271" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB271" t="s">
+      <c r="AA271" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9844,10 +9809,85 @@
       <c r="A272" t="s">
         <v>305</v>
       </c>
+      <c r="B272" t="s">
+        <v>35</v>
+      </c>
+      <c r="D272" t="s">
+        <v>35</v>
+      </c>
       <c r="E272" t="s">
         <v>35</v>
       </c>
+      <c r="F272" t="s">
+        <v>35</v>
+      </c>
+      <c r="G272" t="s">
+        <v>35</v>
+      </c>
+      <c r="H272" t="s">
+        <v>35</v>
+      </c>
+      <c r="I272" t="s">
+        <v>35</v>
+      </c>
+      <c r="L272" t="s">
+        <v>35</v>
+      </c>
+      <c r="M272" t="s">
+        <v>35</v>
+      </c>
+      <c r="N272" t="s">
+        <v>35</v>
+      </c>
+      <c r="O272" t="s">
+        <v>35</v>
+      </c>
+      <c r="P272" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q272" t="s">
+        <v>35</v>
+      </c>
+      <c r="R272" t="s">
+        <v>35</v>
+      </c>
+      <c r="S272" t="s">
+        <v>35</v>
+      </c>
+      <c r="T272" t="s">
+        <v>35</v>
+      </c>
+      <c r="U272" t="s">
+        <v>35</v>
+      </c>
+      <c r="V272" t="s">
+        <v>35</v>
+      </c>
+      <c r="W272" t="s">
+        <v>35</v>
+      </c>
       <c r="AB272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH272" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI272" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9855,10 +9895,10 @@
       <c r="A273" t="s">
         <v>306</v>
       </c>
-      <c r="E273" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB273" t="s">
+      <c r="S273" t="s">
+        <v>35</v>
+      </c>
+      <c r="W273" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9866,13 +9906,7 @@
       <c r="A274" t="s">
         <v>307</v>
       </c>
-      <c r="Y274" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z274" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA274" t="s">
+      <c r="AB274" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9880,7 +9914,10 @@
       <c r="A275" t="s">
         <v>308</v>
       </c>
-      <c r="AC275" t="s">
+      <c r="E275" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB275" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9888,7 +9925,10 @@
       <c r="A276" t="s">
         <v>309</v>
       </c>
-      <c r="AC276" t="s">
+      <c r="E276" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB276" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9896,7 +9936,10 @@
       <c r="A277" t="s">
         <v>310</v>
       </c>
-      <c r="AC277" t="s">
+      <c r="E277" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB277" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9904,7 +9947,13 @@
       <c r="A278" t="s">
         <v>311</v>
       </c>
-      <c r="C278" t="s">
+      <c r="Y278" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z278" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA278" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9912,97 +9961,7 @@
       <c r="A279" t="s">
         <v>312</v>
       </c>
-      <c r="B279" t="s">
-        <v>35</v>
-      </c>
-      <c r="C279" t="s">
-        <v>35</v>
-      </c>
-      <c r="D279" t="s">
-        <v>35</v>
-      </c>
-      <c r="E279" t="s">
-        <v>35</v>
-      </c>
-      <c r="F279" t="s">
-        <v>35</v>
-      </c>
-      <c r="G279" t="s">
-        <v>35</v>
-      </c>
-      <c r="H279" t="s">
-        <v>35</v>
-      </c>
-      <c r="I279" t="s">
-        <v>35</v>
-      </c>
-      <c r="J279" t="s">
-        <v>35</v>
-      </c>
-      <c r="L279" t="s">
-        <v>35</v>
-      </c>
-      <c r="M279" t="s">
-        <v>35</v>
-      </c>
-      <c r="N279" t="s">
-        <v>35</v>
-      </c>
-      <c r="O279" t="s">
-        <v>35</v>
-      </c>
-      <c r="P279" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q279" t="s">
-        <v>35</v>
-      </c>
-      <c r="R279" t="s">
-        <v>35</v>
-      </c>
-      <c r="S279" t="s">
-        <v>35</v>
-      </c>
-      <c r="T279" t="s">
-        <v>35</v>
-      </c>
-      <c r="U279" t="s">
-        <v>35</v>
-      </c>
-      <c r="V279" t="s">
-        <v>35</v>
-      </c>
-      <c r="W279" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y279" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB279" t="s">
-        <v>35</v>
-      </c>
       <c r="AC279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH279" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI279" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10010,7 +9969,7 @@
       <c r="A280" t="s">
         <v>313</v>
       </c>
-      <c r="X280" t="s">
+      <c r="AC280" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10018,7 +9977,7 @@
       <c r="A281" t="s">
         <v>314</v>
       </c>
-      <c r="S281" t="s">
+      <c r="AC281" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10026,7 +9985,7 @@
       <c r="A282" t="s">
         <v>315</v>
       </c>
-      <c r="S282" t="s">
+      <c r="C282" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10034,7 +9993,97 @@
       <c r="A283" t="s">
         <v>316</v>
       </c>
+      <c r="B283" t="s">
+        <v>35</v>
+      </c>
+      <c r="C283" t="s">
+        <v>35</v>
+      </c>
+      <c r="D283" t="s">
+        <v>35</v>
+      </c>
+      <c r="E283" t="s">
+        <v>35</v>
+      </c>
+      <c r="F283" t="s">
+        <v>35</v>
+      </c>
+      <c r="G283" t="s">
+        <v>35</v>
+      </c>
+      <c r="H283" t="s">
+        <v>35</v>
+      </c>
+      <c r="I283" t="s">
+        <v>35</v>
+      </c>
+      <c r="J283" t="s">
+        <v>35</v>
+      </c>
+      <c r="L283" t="s">
+        <v>35</v>
+      </c>
+      <c r="M283" t="s">
+        <v>35</v>
+      </c>
+      <c r="N283" t="s">
+        <v>35</v>
+      </c>
+      <c r="O283" t="s">
+        <v>35</v>
+      </c>
+      <c r="P283" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q283" t="s">
+        <v>35</v>
+      </c>
+      <c r="R283" t="s">
+        <v>35</v>
+      </c>
+      <c r="S283" t="s">
+        <v>35</v>
+      </c>
+      <c r="T283" t="s">
+        <v>35</v>
+      </c>
+      <c r="U283" t="s">
+        <v>35</v>
+      </c>
+      <c r="V283" t="s">
+        <v>35</v>
+      </c>
       <c r="W283" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y283" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH283" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI283" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10042,7 +10091,7 @@
       <c r="A284" t="s">
         <v>317</v>
       </c>
-      <c r="Y284" t="s">
+      <c r="X284" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10050,7 +10099,7 @@
       <c r="A285" t="s">
         <v>318</v>
       </c>
-      <c r="Y285" t="s">
+      <c r="S285" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10058,7 +10107,7 @@
       <c r="A286" t="s">
         <v>319</v>
       </c>
-      <c r="X286" t="s">
+      <c r="S286" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10066,7 +10115,7 @@
       <c r="A287" t="s">
         <v>320</v>
       </c>
-      <c r="X287" t="s">
+      <c r="W287" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10074,7 +10123,7 @@
       <c r="A288" t="s">
         <v>321</v>
       </c>
-      <c r="W288" t="s">
+      <c r="Y288" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10082,7 +10131,7 @@
       <c r="A289" t="s">
         <v>322</v>
       </c>
-      <c r="W289" t="s">
+      <c r="Y289" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10090,10 +10139,7 @@
       <c r="A290" t="s">
         <v>323</v>
       </c>
-      <c r="K290" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y290" t="s">
+      <c r="X290" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10101,10 +10147,45 @@
       <c r="A291" t="s">
         <v>324</v>
       </c>
-      <c r="K291" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y291" t="s">
+      <c r="X291" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="292" spans="1:25">
+      <c r="A292" t="s">
+        <v>325</v>
+      </c>
+      <c r="W292" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="293" spans="1:25">
+      <c r="A293" t="s">
+        <v>326</v>
+      </c>
+      <c r="W293" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="294" spans="1:25">
+      <c r="A294" t="s">
+        <v>327</v>
+      </c>
+      <c r="K294" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y294" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="295" spans="1:25">
+      <c r="A295" t="s">
+        <v>328</v>
+      </c>
+      <c r="K295" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y295" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More updates trying to fix CI
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -4811,9 +4811,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="60"/>
     </xf>
@@ -5127,106 +5126,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the three sample schemas with preparation_condition and storage_method
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2355,11 +2355,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>The condition under which the preparation occurred, such as whether the sample was placed in dry ice during the preparation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A182" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>The model number/name of the instrument used to prepare the sample for the assay</t>
         </r>
       </text>
     </comment>
-    <comment ref="A182" authorId="0">
+    <comment ref="A183" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2372,7 +2385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A183" authorId="0">
+    <comment ref="A184" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2385,7 +2398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A184" authorId="0">
+    <comment ref="A185" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2398,19 +2411,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A185" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The temperature for the preparation process.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A186" authorId="0">
       <text>
         <r>
@@ -3317,7 +3317,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature during storage, after preparation and before the assay is performed.</t>
+          <t>The method by which the sample was stored, after preparation and before the assay was performed.</t>
         </r>
       </text>
     </comment>
@@ -4331,6 +4331,9 @@
     <t>polarity</t>
   </si>
   <si>
+    <t>preparation_condition</t>
+  </si>
+  <si>
     <t>preparation_instrument_model</t>
   </si>
   <si>
@@ -4343,9 +4346,6 @@
     <t>preparation_media</t>
   </si>
   <si>
-    <t>preparation_temperature</t>
-  </si>
-  <si>
     <t>preparation_type</t>
   </si>
   <si>
@@ -4553,7 +4553,7 @@
     <t>storage_media</t>
   </si>
   <si>
-    <t>storage_temperature</t>
+    <t>storage_method</t>
   </si>
   <si>
     <t>suspension_enriched</t>
@@ -8183,22 +8183,13 @@
       <c r="A181" t="s">
         <v>213</v>
       </c>
-      <c r="I181" t="s">
-        <v>34</v>
-      </c>
-      <c r="L181" t="s">
-        <v>34</v>
-      </c>
-      <c r="M181" t="s">
-        <v>34</v>
-      </c>
-      <c r="N181" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q181" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD181" t="s">
+      <c r="X181" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y181" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z181" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8229,7 +8220,22 @@
       <c r="A183" t="s">
         <v>215</v>
       </c>
+      <c r="I183" t="s">
+        <v>34</v>
+      </c>
+      <c r="L183" t="s">
+        <v>34</v>
+      </c>
+      <c r="M183" t="s">
+        <v>34</v>
+      </c>
       <c r="N183" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q183" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD183" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8237,13 +8243,7 @@
       <c r="A184" t="s">
         <v>216</v>
       </c>
-      <c r="X184" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y184" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z184" t="s">
+      <c r="N184" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the three sample schemas with renamed elements (#1185)
* Updated the three sample schemas with preparation_condition and storage_method

* updated sample schemas with preparation condition and sample method

---------

bhonick <bhonick-psc@pop-os.localdomain>
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2355,11 +2355,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>The condition under which the preparation occurred, such as whether the sample was placed in dry ice during the preparation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A182" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>The model number/name of the instrument used to prepare the sample for the assay</t>
         </r>
       </text>
     </comment>
-    <comment ref="A182" authorId="0">
+    <comment ref="A183" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2372,7 +2385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A183" authorId="0">
+    <comment ref="A184" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2385,7 +2398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A184" authorId="0">
+    <comment ref="A185" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2398,19 +2411,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A185" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The temperature for the preparation process.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A186" authorId="0">
       <text>
         <r>
@@ -3317,7 +3317,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature during storage, after preparation and before the assay is performed.</t>
+          <t>The method by which the sample was stored, after preparation and before the assay was performed.</t>
         </r>
       </text>
     </comment>
@@ -4331,6 +4331,9 @@
     <t>polarity</t>
   </si>
   <si>
+    <t>preparation_condition</t>
+  </si>
+  <si>
     <t>preparation_instrument_model</t>
   </si>
   <si>
@@ -4343,9 +4346,6 @@
     <t>preparation_media</t>
   </si>
   <si>
-    <t>preparation_temperature</t>
-  </si>
-  <si>
     <t>preparation_type</t>
   </si>
   <si>
@@ -4553,7 +4553,7 @@
     <t>storage_media</t>
   </si>
   <si>
-    <t>storage_temperature</t>
+    <t>storage_method</t>
   </si>
   <si>
     <t>suspension_enriched</t>
@@ -8183,22 +8183,13 @@
       <c r="A181" t="s">
         <v>213</v>
       </c>
-      <c r="I181" t="s">
-        <v>34</v>
-      </c>
-      <c r="L181" t="s">
-        <v>34</v>
-      </c>
-      <c r="M181" t="s">
-        <v>34</v>
-      </c>
-      <c r="N181" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q181" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD181" t="s">
+      <c r="X181" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y181" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z181" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8229,7 +8220,22 @@
       <c r="A183" t="s">
         <v>215</v>
       </c>
+      <c r="I183" t="s">
+        <v>34</v>
+      </c>
+      <c r="L183" t="s">
+        <v>34</v>
+      </c>
+      <c r="M183" t="s">
+        <v>34</v>
+      </c>
       <c r="N183" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q183" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD183" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8237,13 +8243,7 @@
       <c r="A184" t="s">
         <v>216</v>
       </c>
-      <c r="X184" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y184" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z184" t="s">
+      <c r="N184" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Docs: Add af and stained to is_cedar
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3963,7 +3963,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="340">
   <si>
     <t>af</t>
   </si>
@@ -7092,6 +7092,9 @@
       <c r="A99" t="s">
         <v>134</v>
       </c>
+      <c r="B99" t="s">
+        <v>37</v>
+      </c>
       <c r="L99" t="s">
         <v>37</v>
       </c>
@@ -7105,6 +7108,9 @@
         <v>37</v>
       </c>
       <c r="AC99" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI99" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Docs: Update docs for assays
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3963,7 +3963,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="340">
   <si>
     <t>af</t>
   </si>
@@ -7095,9 +7095,33 @@
       <c r="B99" t="s">
         <v>37</v>
       </c>
+      <c r="E99" t="s">
+        <v>37</v>
+      </c>
+      <c r="F99" t="s">
+        <v>37</v>
+      </c>
+      <c r="G99" t="s">
+        <v>37</v>
+      </c>
+      <c r="I99" t="s">
+        <v>37</v>
+      </c>
       <c r="L99" t="s">
         <v>37</v>
       </c>
+      <c r="O99" t="s">
+        <v>37</v>
+      </c>
+      <c r="P99" t="s">
+        <v>37</v>
+      </c>
+      <c r="R99" t="s">
+        <v>37</v>
+      </c>
+      <c r="U99" t="s">
+        <v>37</v>
+      </c>
       <c r="X99" t="s">
         <v>37</v>
       </c>
@@ -7110,7 +7134,22 @@
       <c r="AC99" t="s">
         <v>37</v>
       </c>
+      <c r="AD99" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE99" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF99" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH99" t="s">
+        <v>37</v>
+      </c>
       <c r="AI99" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK99" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
General: Fixes to address Phil's comments
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3963,7 +3963,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="360">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -7380,15 +7380,6 @@
       <c r="S99" t="s">
         <v>57</v>
       </c>
-      <c r="T99" t="s">
-        <v>57</v>
-      </c>
-      <c r="U99" t="s">
-        <v>57</v>
-      </c>
-      <c r="V99" t="s">
-        <v>57</v>
-      </c>
       <c r="W99" t="s">
         <v>57</v>
       </c>
@@ -7455,16 +7446,10 @@
       <c r="AT99" t="s">
         <v>57</v>
       </c>
-      <c r="AU99" t="s">
-        <v>57</v>
-      </c>
       <c r="AV99" t="s">
         <v>57</v>
       </c>
       <c r="AW99" t="s">
-        <v>57</v>
-      </c>
-      <c r="AX99" t="s">
         <v>57</v>
       </c>
       <c r="AY99" t="s">

</xml_diff>

<commit_message>
Docs: Update docs, fix tests, and update CHANGELG
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3963,7 +3963,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="360">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -6075,6 +6075,9 @@
       <c r="AH21" t="s">
         <v>57</v>
       </c>
+      <c r="AI21" t="s">
+        <v>57</v>
+      </c>
       <c r="AJ21" t="s">
         <v>57</v>
       </c>
@@ -6082,6 +6085,18 @@
         <v>57</v>
       </c>
       <c r="AM21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ21" t="s">
         <v>57</v>
       </c>
       <c r="AR21" t="s">
@@ -6221,6 +6236,9 @@
       <c r="AH22" t="s">
         <v>57</v>
       </c>
+      <c r="AI22" t="s">
+        <v>57</v>
+      </c>
       <c r="AJ22" t="s">
         <v>57</v>
       </c>
@@ -6231,6 +6249,18 @@
         <v>57</v>
       </c>
       <c r="AM22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ22" t="s">
         <v>57</v>
       </c>
       <c r="AR22" t="s">
@@ -7426,6 +7456,9 @@
         <v>57</v>
       </c>
       <c r="AM99" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN99" t="s">
         <v>57</v>
       </c>
       <c r="AO99" t="s">

</xml_diff>

<commit_message>
added URL fields for histology and organ
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2238,7 +2238,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Unique HuBMAP identifier for the organ. This can be found in the Submission ID section of a registered donor on the Ingest UI.</t>
+          <t>UUID or HuBMAP ID of organ</t>
         </r>
       </text>
     </comment>
@@ -2355,11 +2355,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>UUID or HuBMAP ID of parent</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A182" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Further details on organ level QC checks.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A182" authorId="0">
+    <comment ref="A183" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2372,7 +2385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A183" authorId="0">
+    <comment ref="A184" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2385,7 +2398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A184" authorId="0">
+    <comment ref="A185" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2398,7 +2411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A185" authorId="0">
+    <comment ref="A186" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2411,7 +2424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A186" authorId="0">
+    <comment ref="A187" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2424,7 +2437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A187" authorId="0">
+    <comment ref="A188" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2437,7 +2450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A188" authorId="0">
+    <comment ref="A189" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2450,7 +2463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A189" authorId="0">
+    <comment ref="A190" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2463,7 +2476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A190" authorId="0">
+    <comment ref="A191" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2476,7 +2489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A191" authorId="0">
+    <comment ref="A192" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2489,7 +2502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A192" authorId="0">
+    <comment ref="A193" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2502,7 +2515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A193" authorId="0">
+    <comment ref="A194" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2515,7 +2528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A194" authorId="0">
+    <comment ref="A195" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2528,7 +2541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A195" authorId="0">
+    <comment ref="A196" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2541,7 +2554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A196" authorId="0">
+    <comment ref="A197" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2554,7 +2567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A197" authorId="0">
+    <comment ref="A198" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2567,7 +2580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A198" authorId="0">
+    <comment ref="A199" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2580,7 +2593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A199" authorId="0">
+    <comment ref="A200" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2593,7 +2606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A200" authorId="0">
+    <comment ref="A201" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2606,7 +2619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A201" authorId="0">
+    <comment ref="A202" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2619,7 +2632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A202" authorId="0">
+    <comment ref="A203" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2632,7 +2645,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A203" authorId="0">
+    <comment ref="A204" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2645,7 +2658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A204" authorId="0">
+    <comment ref="A205" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2658,7 +2671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A205" authorId="0">
+    <comment ref="A206" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2671,7 +2684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A206" authorId="0">
+    <comment ref="A207" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2684,7 +2697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A207" authorId="0">
+    <comment ref="A208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2697,7 +2710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A208" authorId="0">
+    <comment ref="A209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2710,7 +2723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A209" authorId="0">
+    <comment ref="A210" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2723,7 +2736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A210" authorId="0">
+    <comment ref="A211" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2736,7 +2749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A211" authorId="0">
+    <comment ref="A212" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2749,7 +2762,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A212" authorId="0">
+    <comment ref="A213" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2762,7 +2775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A213" authorId="0">
+    <comment ref="A214" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2775,7 +2788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A214" authorId="0">
+    <comment ref="A215" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2788,7 +2801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A215" authorId="0">
+    <comment ref="A216" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2801,7 +2814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A216" authorId="0">
+    <comment ref="A217" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2814,7 +2827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A217" authorId="0">
+    <comment ref="A218" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2827,7 +2840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A218" authorId="0">
+    <comment ref="A219" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2840,7 +2853,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A219" authorId="0">
+    <comment ref="A220" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2853,7 +2866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A220" authorId="0">
+    <comment ref="A221" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2866,7 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A221" authorId="0">
+    <comment ref="A222" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2892,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A222" authorId="0">
+    <comment ref="A223" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2892,7 +2905,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A223" authorId="0">
+    <comment ref="A224" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2905,7 +2918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A224" authorId="0">
+    <comment ref="A225" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2918,7 +2931,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A225" authorId="0">
+    <comment ref="A226" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2931,7 +2944,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A226" authorId="0">
+    <comment ref="A227" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2944,7 +2957,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A227" authorId="0">
+    <comment ref="A228" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2957,7 +2970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A228" authorId="0">
+    <comment ref="A229" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2970,7 +2983,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A229" authorId="0">
+    <comment ref="A230" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2983,7 +2996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A230" authorId="0">
+    <comment ref="A231" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2996,7 +3009,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A231" authorId="0">
+    <comment ref="A232" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3009,7 +3022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A232" authorId="0">
+    <comment ref="A233" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3022,7 +3035,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A233" authorId="0">
+    <comment ref="A234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3035,7 +3048,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A234" authorId="0">
+    <comment ref="A235" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3048,7 +3061,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A235" authorId="0">
+    <comment ref="A236" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3061,7 +3074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A236" authorId="0">
+    <comment ref="A237" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3074,7 +3087,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A237" authorId="0">
+    <comment ref="A238" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3087,7 +3100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A238" authorId="0">
+    <comment ref="A239" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3100,7 +3113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A239" authorId="0">
+    <comment ref="A240" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3113,7 +3126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A240" authorId="0">
+    <comment ref="A241" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3126,7 +3139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A241" authorId="0">
+    <comment ref="A242" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3139,7 +3152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A242" authorId="0">
+    <comment ref="A243" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3152,7 +3165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A243" authorId="0">
+    <comment ref="A244" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3165,7 +3178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A244" authorId="0">
+    <comment ref="A245" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3178,7 +3191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A245" authorId="0">
+    <comment ref="A246" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3191,7 +3204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A246" authorId="0">
+    <comment ref="A247" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3204,7 +3217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A247" authorId="0">
+    <comment ref="A248" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3217,7 +3230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A248" authorId="0">
+    <comment ref="A249" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3230,7 +3243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A249" authorId="0">
+    <comment ref="A250" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3243,7 +3256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A250" authorId="0">
+    <comment ref="A251" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3256,7 +3269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A251" authorId="0">
+    <comment ref="A252" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3269,7 +3282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A252" authorId="0">
+    <comment ref="A253" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3282,7 +3295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A253" authorId="0">
+    <comment ref="A254" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3295,7 +3308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A254" authorId="0">
+    <comment ref="A255" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3308,7 +3321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A255" authorId="0">
+    <comment ref="A256" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3321,7 +3334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A256" authorId="0">
+    <comment ref="A257" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3334,7 +3347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A257" authorId="0">
+    <comment ref="A258" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3347,7 +3360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A258" authorId="0">
+    <comment ref="A259" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3360,7 +3373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A259" authorId="0">
+    <comment ref="A260" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3373,7 +3386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A260" authorId="0">
+    <comment ref="A261" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3386,7 +3399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A261" authorId="0">
+    <comment ref="A262" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3399,7 +3412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A262" authorId="0">
+    <comment ref="A263" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3412,7 +3425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A263" authorId="0">
+    <comment ref="A264" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3425,7 +3438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A264" authorId="0">
+    <comment ref="A265" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3438,7 +3451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A265" authorId="0">
+    <comment ref="A266" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3451,7 +3464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A266" authorId="0">
+    <comment ref="A267" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3464,7 +3477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A267" authorId="0">
+    <comment ref="A268" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3477,7 +3490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A268" authorId="0">
+    <comment ref="A269" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3490,7 +3503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A269" authorId="0">
+    <comment ref="A270" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3503,7 +3516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A270" authorId="0">
+    <comment ref="A271" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3516,7 +3529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A271" authorId="0">
+    <comment ref="A272" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3529,7 +3542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A272" authorId="0">
+    <comment ref="A273" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3542,7 +3555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A273" authorId="0">
+    <comment ref="A274" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3555,7 +3568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A274" authorId="0">
+    <comment ref="A275" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3568,7 +3581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A275" authorId="0">
+    <comment ref="A276" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3581,7 +3594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A276" authorId="0">
+    <comment ref="A277" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3594,7 +3607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A277" authorId="0">
+    <comment ref="A278" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3607,7 +3620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A278" authorId="0">
+    <comment ref="A279" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3620,7 +3633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A279" authorId="0">
+    <comment ref="A280" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3633,7 +3646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A280" authorId="0">
+    <comment ref="A281" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3646,7 +3659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A281" authorId="0">
+    <comment ref="A282" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3659,7 +3672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A282" authorId="0">
+    <comment ref="A283" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3672,7 +3685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A283" authorId="0">
+    <comment ref="A284" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3685,7 +3698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A284" authorId="0">
+    <comment ref="A285" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3698,7 +3711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A285" authorId="0">
+    <comment ref="A286" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3711,7 +3724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A286" authorId="0">
+    <comment ref="A287" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3724,7 +3737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A287" authorId="0">
+    <comment ref="A288" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3737,7 +3750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A288" authorId="0">
+    <comment ref="A289" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3750,7 +3763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A289" authorId="0">
+    <comment ref="A290" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3763,7 +3776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A290" authorId="0">
+    <comment ref="A291" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3776,7 +3789,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A291" authorId="0">
+    <comment ref="A292" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3789,7 +3802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A292" authorId="0">
+    <comment ref="A293" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3802,7 +3815,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A293" authorId="0">
+    <comment ref="A294" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3815,7 +3828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A294" authorId="0">
+    <comment ref="A295" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3828,7 +3841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A295" authorId="0">
+    <comment ref="A296" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3841,7 +3854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A296" authorId="0">
+    <comment ref="A297" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3854,7 +3867,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A297" authorId="0">
+    <comment ref="A298" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3867,7 +3880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A298" authorId="0">
+    <comment ref="A299" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3880,7 +3893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A299" authorId="0">
+    <comment ref="A300" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3893,7 +3906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A300" authorId="0">
+    <comment ref="A301" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3906,7 +3919,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A301" authorId="0">
+    <comment ref="A302" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3919,7 +3932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A302" authorId="0">
+    <comment ref="A303" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3932,7 +3945,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A303" authorId="0">
+    <comment ref="A304" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3945,7 +3958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A304" authorId="0">
+    <comment ref="A305" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3963,7 +3976,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="362">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -4674,6 +4687,9 @@
   </si>
   <si>
     <t>overall_protocols_io_doi</t>
+  </si>
+  <si>
+    <t>parent_id</t>
   </si>
   <si>
     <t>pathologist_report</t>
@@ -5386,7 +5402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF304"/>
+  <dimension ref="A1:BF305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -8804,7 +8820,7 @@
       <c r="A181" t="s">
         <v>237</v>
       </c>
-      <c r="AP181" t="s">
+      <c r="U181" t="s">
         <v>58</v>
       </c>
     </row>
@@ -8812,7 +8828,7 @@
       <c r="A182" t="s">
         <v>238</v>
       </c>
-      <c r="AQ182" t="s">
+      <c r="AP182" t="s">
         <v>58</v>
       </c>
     </row>
@@ -8828,7 +8844,7 @@
       <c r="A184" t="s">
         <v>240</v>
       </c>
-      <c r="AK184" t="s">
+      <c r="AQ184" t="s">
         <v>58</v>
       </c>
     </row>
@@ -8839,93 +8855,15 @@
       <c r="AK185" t="s">
         <v>58</v>
       </c>
-      <c r="AP185" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="186" spans="1:57">
       <c r="A186" t="s">
         <v>242</v>
       </c>
-      <c r="C186" t="s">
-        <v>58</v>
-      </c>
-      <c r="E186" t="s">
-        <v>58</v>
-      </c>
-      <c r="F186" t="s">
-        <v>58</v>
-      </c>
-      <c r="G186" t="s">
-        <v>58</v>
-      </c>
-      <c r="H186" t="s">
-        <v>58</v>
-      </c>
-      <c r="I186" t="s">
-        <v>58</v>
-      </c>
-      <c r="J186" t="s">
-        <v>58</v>
-      </c>
-      <c r="R186" t="s">
-        <v>58</v>
-      </c>
-      <c r="V186" t="s">
-        <v>58</v>
-      </c>
-      <c r="W186" t="s">
-        <v>58</v>
-      </c>
-      <c r="X186" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y186" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX186" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ186" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA186" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC186" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE186" t="s">
+      <c r="AK186" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP186" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9019,7 +8957,85 @@
       <c r="A188" t="s">
         <v>244</v>
       </c>
+      <c r="C188" t="s">
+        <v>58</v>
+      </c>
+      <c r="E188" t="s">
+        <v>58</v>
+      </c>
+      <c r="F188" t="s">
+        <v>58</v>
+      </c>
+      <c r="G188" t="s">
+        <v>58</v>
+      </c>
+      <c r="H188" t="s">
+        <v>58</v>
+      </c>
+      <c r="I188" t="s">
+        <v>58</v>
+      </c>
+      <c r="J188" t="s">
+        <v>58</v>
+      </c>
+      <c r="R188" t="s">
+        <v>58</v>
+      </c>
+      <c r="V188" t="s">
+        <v>58</v>
+      </c>
+      <c r="W188" t="s">
+        <v>58</v>
+      </c>
+      <c r="X188" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y188" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z188" t="s">
+        <v>58</v>
+      </c>
       <c r="AD188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX188" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ188" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA188" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC188" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE188" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9067,19 +9083,7 @@
       <c r="A194" t="s">
         <v>250</v>
       </c>
-      <c r="E194" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE194" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF194" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ194" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC194" t="s">
+      <c r="AD194" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9107,19 +9111,19 @@
       <c r="A196" t="s">
         <v>252</v>
       </c>
-      <c r="I196" t="s">
-        <v>58</v>
-      </c>
-      <c r="R196" t="s">
-        <v>58</v>
-      </c>
-      <c r="X196" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y196" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH196" t="s">
+      <c r="E196" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE196" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF196" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ196" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC196" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9127,13 +9131,19 @@
       <c r="A197" t="s">
         <v>253</v>
       </c>
-      <c r="AQ197" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR197" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS197" t="s">
+      <c r="I197" t="s">
+        <v>58</v>
+      </c>
+      <c r="R197" t="s">
+        <v>58</v>
+      </c>
+      <c r="X197" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y197" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH197" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9141,22 +9151,13 @@
       <c r="A198" t="s">
         <v>254</v>
       </c>
-      <c r="J198" t="s">
-        <v>58</v>
-      </c>
-      <c r="V198" t="s">
-        <v>58</v>
-      </c>
-      <c r="W198" t="s">
-        <v>58</v>
-      </c>
-      <c r="X198" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD198" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX198" t="s">
+      <c r="AQ198" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR198" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS198" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9187,7 +9188,22 @@
       <c r="A200" t="s">
         <v>256</v>
       </c>
+      <c r="J200" t="s">
+        <v>58</v>
+      </c>
+      <c r="V200" t="s">
+        <v>58</v>
+      </c>
+      <c r="W200" t="s">
+        <v>58</v>
+      </c>
       <c r="X200" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD200" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX200" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9195,13 +9211,7 @@
       <c r="A201" t="s">
         <v>257</v>
       </c>
-      <c r="AQ201" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR201" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS201" t="s">
+      <c r="X201" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9209,7 +9219,13 @@
       <c r="A202" t="s">
         <v>258</v>
       </c>
-      <c r="X202" t="s">
+      <c r="AQ202" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR202" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS202" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9217,7 +9233,7 @@
       <c r="A203" t="s">
         <v>259</v>
       </c>
-      <c r="AD203" t="s">
+      <c r="X203" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9241,7 +9257,7 @@
       <c r="A206" t="s">
         <v>262</v>
       </c>
-      <c r="BC206" t="s">
+      <c r="AD206" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9249,7 +9265,7 @@
       <c r="A207" t="s">
         <v>263</v>
       </c>
-      <c r="AP207" t="s">
+      <c r="BC207" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9257,19 +9273,7 @@
       <c r="A208" t="s">
         <v>264</v>
       </c>
-      <c r="H208" t="s">
-        <v>58</v>
-      </c>
-      <c r="I208" t="s">
-        <v>58</v>
-      </c>
-      <c r="X208" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y208" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH208" t="s">
+      <c r="AP208" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9277,13 +9281,19 @@
       <c r="A209" t="s">
         <v>265</v>
       </c>
+      <c r="H209" t="s">
+        <v>58</v>
+      </c>
       <c r="I209" t="s">
         <v>58</v>
       </c>
-      <c r="R209" t="s">
+      <c r="X209" t="s">
         <v>58</v>
       </c>
       <c r="Y209" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH209" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9291,13 +9301,13 @@
       <c r="A210" t="s">
         <v>266</v>
       </c>
-      <c r="AQ210" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR210" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS210" t="s">
+      <c r="I210" t="s">
+        <v>58</v>
+      </c>
+      <c r="R210" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y210" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9319,85 +9329,13 @@
       <c r="A212" t="s">
         <v>268</v>
       </c>
-      <c r="C212" t="s">
-        <v>58</v>
-      </c>
-      <c r="E212" t="s">
-        <v>58</v>
-      </c>
-      <c r="F212" t="s">
-        <v>58</v>
-      </c>
-      <c r="G212" t="s">
-        <v>58</v>
-      </c>
-      <c r="H212" t="s">
-        <v>58</v>
-      </c>
-      <c r="I212" t="s">
-        <v>58</v>
-      </c>
-      <c r="J212" t="s">
-        <v>58</v>
-      </c>
-      <c r="R212" t="s">
-        <v>58</v>
-      </c>
-      <c r="V212" t="s">
-        <v>58</v>
-      </c>
-      <c r="W212" t="s">
-        <v>58</v>
-      </c>
-      <c r="X212" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y212" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX212" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ212" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA212" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC212" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE212" t="s">
+      <c r="AQ212" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR212" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS212" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9405,7 +9343,85 @@
       <c r="A213" t="s">
         <v>269</v>
       </c>
+      <c r="C213" t="s">
+        <v>58</v>
+      </c>
+      <c r="E213" t="s">
+        <v>58</v>
+      </c>
+      <c r="F213" t="s">
+        <v>58</v>
+      </c>
+      <c r="G213" t="s">
+        <v>58</v>
+      </c>
+      <c r="H213" t="s">
+        <v>58</v>
+      </c>
+      <c r="I213" t="s">
+        <v>58</v>
+      </c>
+      <c r="J213" t="s">
+        <v>58</v>
+      </c>
+      <c r="R213" t="s">
+        <v>58</v>
+      </c>
+      <c r="V213" t="s">
+        <v>58</v>
+      </c>
+      <c r="W213" t="s">
+        <v>58</v>
+      </c>
+      <c r="X213" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y213" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX213" t="s">
+        <v>58</v>
+      </c>
       <c r="AZ213" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA213" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC213" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE213" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9413,13 +9429,7 @@
       <c r="A214" t="s">
         <v>270</v>
       </c>
-      <c r="AQ214" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR214" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS214" t="s">
+      <c r="AZ214" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9427,7 +9437,13 @@
       <c r="A215" t="s">
         <v>271</v>
       </c>
-      <c r="BC215" t="s">
+      <c r="AQ215" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR215" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS215" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9435,7 +9451,7 @@
       <c r="A216" t="s">
         <v>272</v>
       </c>
-      <c r="Z216" t="s">
+      <c r="BC216" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9451,22 +9467,7 @@
       <c r="A218" t="s">
         <v>274</v>
       </c>
-      <c r="J218" t="s">
-        <v>58</v>
-      </c>
-      <c r="V218" t="s">
-        <v>58</v>
-      </c>
-      <c r="W218" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD218" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG218" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX218" t="s">
+      <c r="Z218" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9474,7 +9475,22 @@
       <c r="A219" t="s">
         <v>275</v>
       </c>
-      <c r="AF219" t="s">
+      <c r="J219" t="s">
+        <v>58</v>
+      </c>
+      <c r="V219" t="s">
+        <v>58</v>
+      </c>
+      <c r="W219" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD219" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG219" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX219" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9482,58 +9498,7 @@
       <c r="A220" t="s">
         <v>276</v>
       </c>
-      <c r="C220" t="s">
-        <v>58</v>
-      </c>
-      <c r="E220" t="s">
-        <v>58</v>
-      </c>
-      <c r="H220" t="s">
-        <v>58</v>
-      </c>
-      <c r="I220" t="s">
-        <v>58</v>
-      </c>
-      <c r="J220" t="s">
-        <v>58</v>
-      </c>
-      <c r="R220" t="s">
-        <v>58</v>
-      </c>
-      <c r="X220" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y220" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z220" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD220" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE220" t="s">
-        <v>58</v>
-      </c>
       <c r="AF220" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG220" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH220" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ220" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX220" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA220" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC220" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9724,16 +9689,40 @@
       <c r="E224" t="s">
         <v>58</v>
       </c>
+      <c r="H224" t="s">
+        <v>58</v>
+      </c>
+      <c r="I224" t="s">
+        <v>58</v>
+      </c>
       <c r="J224" t="s">
         <v>58</v>
       </c>
+      <c r="R224" t="s">
+        <v>58</v>
+      </c>
+      <c r="X224" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y224" t="s">
+        <v>58</v>
+      </c>
       <c r="Z224" t="s">
         <v>58</v>
       </c>
+      <c r="AD224" t="s">
+        <v>58</v>
+      </c>
       <c r="AE224" t="s">
         <v>58</v>
       </c>
       <c r="AF224" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG224" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH224" t="s">
         <v>58</v>
       </c>
       <c r="AJ224" t="s">
@@ -9788,10 +9777,34 @@
       <c r="A226" t="s">
         <v>282</v>
       </c>
-      <c r="AU226" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV226" t="s">
+      <c r="C226" t="s">
+        <v>58</v>
+      </c>
+      <c r="E226" t="s">
+        <v>58</v>
+      </c>
+      <c r="J226" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z226" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE226" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF226" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ226" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX226" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA226" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC226" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9799,7 +9812,10 @@
       <c r="A227" t="s">
         <v>283</v>
       </c>
-      <c r="G227" t="s">
+      <c r="AU227" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV227" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9818,42 +9834,21 @@
       <c r="G229" t="s">
         <v>58</v>
       </c>
-      <c r="AU229" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV229" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ229" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="230" spans="1:55">
       <c r="A230" t="s">
         <v>286</v>
       </c>
-      <c r="E230" t="s">
-        <v>58</v>
-      </c>
-      <c r="V230" t="s">
-        <v>58</v>
-      </c>
-      <c r="W230" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD230" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE230" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF230" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ230" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC230" t="s">
+      <c r="G230" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU230" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV230" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ230" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9890,7 +9885,28 @@
       <c r="A232" t="s">
         <v>288</v>
       </c>
-      <c r="D232" t="s">
+      <c r="E232" t="s">
+        <v>58</v>
+      </c>
+      <c r="V232" t="s">
+        <v>58</v>
+      </c>
+      <c r="W232" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD232" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE232" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF232" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ232" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC232" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9898,16 +9914,7 @@
       <c r="A233" t="s">
         <v>289</v>
       </c>
-      <c r="AP233" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ233" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR233" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS233" t="s">
+      <c r="D233" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9915,7 +9922,16 @@
       <c r="A234" t="s">
         <v>290</v>
       </c>
-      <c r="F234" t="s">
+      <c r="AP234" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ234" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR234" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS234" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9923,13 +9939,7 @@
       <c r="A235" t="s">
         <v>291</v>
       </c>
-      <c r="AT235" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU235" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV235" t="s">
+      <c r="F235" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10007,7 +10017,13 @@
       <c r="A241" t="s">
         <v>297</v>
       </c>
-      <c r="AF241" t="s">
+      <c r="AT241" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU241" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV241" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10015,7 +10031,7 @@
       <c r="A242" t="s">
         <v>298</v>
       </c>
-      <c r="AR242" t="s">
+      <c r="AF242" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10023,37 +10039,7 @@
       <c r="A243" t="s">
         <v>299</v>
       </c>
-      <c r="I243" t="s">
-        <v>58</v>
-      </c>
-      <c r="J243" t="s">
-        <v>58</v>
-      </c>
-      <c r="R243" t="s">
-        <v>58</v>
-      </c>
-      <c r="V243" t="s">
-        <v>58</v>
-      </c>
-      <c r="W243" t="s">
-        <v>58</v>
-      </c>
-      <c r="X243" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y243" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD243" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG243" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX243" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA243" t="s">
+      <c r="AR243" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10061,7 +10047,37 @@
       <c r="A244" t="s">
         <v>300</v>
       </c>
-      <c r="AR244" t="s">
+      <c r="I244" t="s">
+        <v>58</v>
+      </c>
+      <c r="J244" t="s">
+        <v>58</v>
+      </c>
+      <c r="R244" t="s">
+        <v>58</v>
+      </c>
+      <c r="V244" t="s">
+        <v>58</v>
+      </c>
+      <c r="W244" t="s">
+        <v>58</v>
+      </c>
+      <c r="X244" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y244" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD244" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG244" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX244" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA244" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10077,13 +10093,7 @@
       <c r="A246" t="s">
         <v>302</v>
       </c>
-      <c r="V246" t="s">
-        <v>58</v>
-      </c>
-      <c r="W246" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD246" t="s">
+      <c r="AR246" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10091,7 +10101,13 @@
       <c r="A247" t="s">
         <v>303</v>
       </c>
-      <c r="AF247" t="s">
+      <c r="V247" t="s">
+        <v>58</v>
+      </c>
+      <c r="W247" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD247" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10099,25 +10115,7 @@
       <c r="A248" t="s">
         <v>304</v>
       </c>
-      <c r="F248" t="s">
-        <v>58</v>
-      </c>
-      <c r="G248" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT248" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU248" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV248" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ248" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE248" t="s">
+      <c r="AF248" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10203,13 +10201,25 @@
       <c r="A252" t="s">
         <v>308</v>
       </c>
-      <c r="V252" t="s">
-        <v>58</v>
-      </c>
-      <c r="W252" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD252" t="s">
+      <c r="F252" t="s">
+        <v>58</v>
+      </c>
+      <c r="G252" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT252" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU252" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV252" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ252" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE252" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10217,19 +10227,13 @@
       <c r="A253" t="s">
         <v>309</v>
       </c>
-      <c r="E253" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE253" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF253" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ253" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC253" t="s">
+      <c r="V253" t="s">
+        <v>58</v>
+      </c>
+      <c r="W253" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD253" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10237,7 +10241,19 @@
       <c r="A254" t="s">
         <v>310</v>
       </c>
+      <c r="E254" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE254" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF254" t="s">
+        <v>58</v>
+      </c>
       <c r="AJ254" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC254" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10253,7 +10269,7 @@
       <c r="A256" t="s">
         <v>312</v>
       </c>
-      <c r="AV256" t="s">
+      <c r="AJ256" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10261,13 +10277,7 @@
       <c r="A257" t="s">
         <v>313</v>
       </c>
-      <c r="AQ257" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR257" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS257" t="s">
+      <c r="AV257" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10289,13 +10299,13 @@
       <c r="A259" t="s">
         <v>315</v>
       </c>
-      <c r="I259" t="s">
-        <v>58</v>
-      </c>
-      <c r="R259" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y259" t="s">
+      <c r="AQ259" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR259" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS259" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10331,7 +10341,13 @@
       <c r="A262" t="s">
         <v>318</v>
       </c>
-      <c r="AP262" t="s">
+      <c r="I262" t="s">
+        <v>58</v>
+      </c>
+      <c r="R262" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y262" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10363,7 +10379,7 @@
       <c r="A266" t="s">
         <v>322</v>
       </c>
-      <c r="BC266" t="s">
+      <c r="AP266" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10371,7 +10387,7 @@
       <c r="A267" t="s">
         <v>323</v>
       </c>
-      <c r="BA267" t="s">
+      <c r="BC267" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10379,10 +10395,7 @@
       <c r="A268" t="s">
         <v>324</v>
       </c>
-      <c r="V268" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD268" t="s">
+      <c r="BA268" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10390,7 +10403,10 @@
       <c r="A269" t="s">
         <v>325</v>
       </c>
-      <c r="Z269" t="s">
+      <c r="V269" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD269" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10398,13 +10414,7 @@
       <c r="A270" t="s">
         <v>326</v>
       </c>
-      <c r="AQ270" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR270" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS270" t="s">
+      <c r="Z270" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10426,6 +10436,12 @@
       <c r="A272" t="s">
         <v>328</v>
       </c>
+      <c r="AQ272" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR272" t="s">
+        <v>58</v>
+      </c>
       <c r="AS272" t="s">
         <v>58</v>
       </c>
@@ -10458,85 +10474,7 @@
       <c r="A276" t="s">
         <v>332</v>
       </c>
-      <c r="C276" t="s">
-        <v>58</v>
-      </c>
-      <c r="E276" t="s">
-        <v>58</v>
-      </c>
-      <c r="F276" t="s">
-        <v>58</v>
-      </c>
-      <c r="G276" t="s">
-        <v>58</v>
-      </c>
-      <c r="H276" t="s">
-        <v>58</v>
-      </c>
-      <c r="I276" t="s">
-        <v>58</v>
-      </c>
-      <c r="J276" t="s">
-        <v>58</v>
-      </c>
-      <c r="R276" t="s">
-        <v>58</v>
-      </c>
-      <c r="V276" t="s">
-        <v>58</v>
-      </c>
-      <c r="W276" t="s">
-        <v>58</v>
-      </c>
-      <c r="X276" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y276" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX276" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ276" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA276" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC276" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE276" t="s">
+      <c r="AS276" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10544,7 +10482,85 @@
       <c r="A277" t="s">
         <v>333</v>
       </c>
-      <c r="AK277" t="s">
+      <c r="C277" t="s">
+        <v>58</v>
+      </c>
+      <c r="E277" t="s">
+        <v>58</v>
+      </c>
+      <c r="F277" t="s">
+        <v>58</v>
+      </c>
+      <c r="G277" t="s">
+        <v>58</v>
+      </c>
+      <c r="H277" t="s">
+        <v>58</v>
+      </c>
+      <c r="I277" t="s">
+        <v>58</v>
+      </c>
+      <c r="J277" t="s">
+        <v>58</v>
+      </c>
+      <c r="R277" t="s">
+        <v>58</v>
+      </c>
+      <c r="V277" t="s">
+        <v>58</v>
+      </c>
+      <c r="W277" t="s">
+        <v>58</v>
+      </c>
+      <c r="X277" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y277" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX277" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ277" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA277" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC277" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE277" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10560,10 +10576,7 @@
       <c r="A279" t="s">
         <v>335</v>
       </c>
-      <c r="AE279" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ279" t="s">
+      <c r="AK279" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10571,7 +10584,10 @@
       <c r="A280" t="s">
         <v>336</v>
       </c>
-      <c r="AK280" t="s">
+      <c r="AE280" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ280" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10579,7 +10595,7 @@
       <c r="A281" t="s">
         <v>337</v>
       </c>
-      <c r="AT281" t="s">
+      <c r="AK281" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10587,9 +10603,6 @@
       <c r="A282" t="s">
         <v>338</v>
       </c>
-      <c r="F282" t="s">
-        <v>58</v>
-      </c>
       <c r="AT282" t="s">
         <v>58</v>
       </c>
@@ -10620,13 +10633,10 @@
       <c r="A285" t="s">
         <v>341</v>
       </c>
-      <c r="AQ285" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR285" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS285" t="s">
+      <c r="F285" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT285" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10634,7 +10644,13 @@
       <c r="A286" t="s">
         <v>342</v>
       </c>
-      <c r="AU286" t="s">
+      <c r="AQ286" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR286" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS286" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10658,7 +10674,7 @@
       <c r="A289" t="s">
         <v>345</v>
       </c>
-      <c r="D289" t="s">
+      <c r="AU289" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10666,100 +10682,7 @@
       <c r="A290" t="s">
         <v>346</v>
       </c>
-      <c r="C290" t="s">
-        <v>58</v>
-      </c>
       <c r="D290" t="s">
-        <v>58</v>
-      </c>
-      <c r="E290" t="s">
-        <v>58</v>
-      </c>
-      <c r="F290" t="s">
-        <v>58</v>
-      </c>
-      <c r="G290" t="s">
-        <v>58</v>
-      </c>
-      <c r="H290" t="s">
-        <v>58</v>
-      </c>
-      <c r="I290" t="s">
-        <v>58</v>
-      </c>
-      <c r="J290" t="s">
-        <v>58</v>
-      </c>
-      <c r="L290" t="s">
-        <v>58</v>
-      </c>
-      <c r="R290" t="s">
-        <v>58</v>
-      </c>
-      <c r="V290" t="s">
-        <v>58</v>
-      </c>
-      <c r="W290" t="s">
-        <v>58</v>
-      </c>
-      <c r="X290" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y290" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX290" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ290" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA290" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC290" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE290" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10767,7 +10690,100 @@
       <c r="A291" t="s">
         <v>347</v>
       </c>
-      <c r="AP291" t="s">
+      <c r="C291" t="s">
+        <v>58</v>
+      </c>
+      <c r="D291" t="s">
+        <v>58</v>
+      </c>
+      <c r="E291" t="s">
+        <v>58</v>
+      </c>
+      <c r="F291" t="s">
+        <v>58</v>
+      </c>
+      <c r="G291" t="s">
+        <v>58</v>
+      </c>
+      <c r="H291" t="s">
+        <v>58</v>
+      </c>
+      <c r="I291" t="s">
+        <v>58</v>
+      </c>
+      <c r="J291" t="s">
+        <v>58</v>
+      </c>
+      <c r="L291" t="s">
+        <v>58</v>
+      </c>
+      <c r="R291" t="s">
+        <v>58</v>
+      </c>
+      <c r="V291" t="s">
+        <v>58</v>
+      </c>
+      <c r="W291" t="s">
+        <v>58</v>
+      </c>
+      <c r="X291" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y291" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX291" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ291" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA291" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC291" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE291" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10775,7 +10791,7 @@
       <c r="A292" t="s">
         <v>348</v>
       </c>
-      <c r="AE292" t="s">
+      <c r="AP292" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10791,7 +10807,7 @@
       <c r="A294" t="s">
         <v>350</v>
       </c>
-      <c r="AJ294" t="s">
+      <c r="AE294" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10799,7 +10815,7 @@
       <c r="A295" t="s">
         <v>351</v>
       </c>
-      <c r="AQ295" t="s">
+      <c r="AJ295" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10815,7 +10831,7 @@
       <c r="A297" t="s">
         <v>353</v>
       </c>
-      <c r="AP297" t="s">
+      <c r="AQ297" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10831,7 +10847,7 @@
       <c r="A299" t="s">
         <v>355</v>
       </c>
-      <c r="AK299" t="s">
+      <c r="AP299" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10847,7 +10863,7 @@
       <c r="A301" t="s">
         <v>357</v>
       </c>
-      <c r="AJ301" t="s">
+      <c r="AK301" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10863,10 +10879,7 @@
       <c r="A303" t="s">
         <v>359</v>
       </c>
-      <c r="AK303" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ303" t="s">
+      <c r="AJ303" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10874,7 +10887,18 @@
       <c r="A304" t="s">
         <v>360</v>
       </c>
+      <c r="AK304" t="s">
+        <v>58</v>
+      </c>
       <c r="AQ304" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="305" spans="1:43">
+      <c r="A305" t="s">
+        <v>361</v>
+      </c>
+      <c r="AQ305" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
forgot to run general test file again, needed to fix docs
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2368,11 +2368,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>UUID or HuBMAP ID of parent</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A183" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Further details on organ level QC checks.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A183" authorId="0">
+    <comment ref="A184" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2385,7 +2398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A184" authorId="0">
+    <comment ref="A185" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2398,7 +2411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A185" authorId="0">
+    <comment ref="A186" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2411,7 +2424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A186" authorId="0">
+    <comment ref="A187" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2424,7 +2437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A187" authorId="0">
+    <comment ref="A188" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2437,7 +2450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A188" authorId="0">
+    <comment ref="A189" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2450,7 +2463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A189" authorId="0">
+    <comment ref="A190" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2463,7 +2476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A190" authorId="0">
+    <comment ref="A191" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2476,7 +2489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A191" authorId="0">
+    <comment ref="A192" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2489,7 +2502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A192" authorId="0">
+    <comment ref="A193" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2502,7 +2515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A193" authorId="0">
+    <comment ref="A194" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2515,7 +2528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A194" authorId="0">
+    <comment ref="A195" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2528,7 +2541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A195" authorId="0">
+    <comment ref="A196" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2541,7 +2554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A196" authorId="0">
+    <comment ref="A197" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2554,7 +2567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A197" authorId="0">
+    <comment ref="A198" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2567,7 +2580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A198" authorId="0">
+    <comment ref="A199" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2580,7 +2593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A199" authorId="0">
+    <comment ref="A200" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2593,7 +2606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A200" authorId="0">
+    <comment ref="A201" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2606,7 +2619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A201" authorId="0">
+    <comment ref="A202" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2619,7 +2632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A202" authorId="0">
+    <comment ref="A203" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2632,7 +2645,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A203" authorId="0">
+    <comment ref="A204" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2645,7 +2658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A204" authorId="0">
+    <comment ref="A205" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2658,7 +2671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A205" authorId="0">
+    <comment ref="A206" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2671,7 +2684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A206" authorId="0">
+    <comment ref="A207" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2684,7 +2697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A207" authorId="0">
+    <comment ref="A208" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2697,7 +2710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A208" authorId="0">
+    <comment ref="A209" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2710,7 +2723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A209" authorId="0">
+    <comment ref="A210" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2723,7 +2736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A210" authorId="0">
+    <comment ref="A211" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2736,7 +2749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A211" authorId="0">
+    <comment ref="A212" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2749,7 +2762,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A212" authorId="0">
+    <comment ref="A213" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2762,7 +2775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A213" authorId="0">
+    <comment ref="A214" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2775,7 +2788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A214" authorId="0">
+    <comment ref="A215" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2788,7 +2801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A215" authorId="0">
+    <comment ref="A216" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2801,7 +2814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A216" authorId="0">
+    <comment ref="A217" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2814,7 +2827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A217" authorId="0">
+    <comment ref="A218" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2827,7 +2840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A218" authorId="0">
+    <comment ref="A219" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2840,7 +2853,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A219" authorId="0">
+    <comment ref="A220" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2853,7 +2866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A220" authorId="0">
+    <comment ref="A221" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2866,7 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A221" authorId="0">
+    <comment ref="A222" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2892,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A222" authorId="0">
+    <comment ref="A223" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2892,7 +2905,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A223" authorId="0">
+    <comment ref="A224" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2905,7 +2918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A224" authorId="0">
+    <comment ref="A225" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2918,7 +2931,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A225" authorId="0">
+    <comment ref="A226" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2931,7 +2944,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A226" authorId="0">
+    <comment ref="A227" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2944,7 +2957,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A227" authorId="0">
+    <comment ref="A228" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2957,7 +2970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A228" authorId="0">
+    <comment ref="A229" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2970,7 +2983,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A229" authorId="0">
+    <comment ref="A230" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2983,7 +2996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A230" authorId="0">
+    <comment ref="A231" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2996,7 +3009,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A231" authorId="0">
+    <comment ref="A232" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3009,7 +3022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A232" authorId="0">
+    <comment ref="A233" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3022,7 +3035,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A233" authorId="0">
+    <comment ref="A234" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3035,7 +3048,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A234" authorId="0">
+    <comment ref="A235" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3048,7 +3061,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A235" authorId="0">
+    <comment ref="A236" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3061,7 +3074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A236" authorId="0">
+    <comment ref="A237" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3074,7 +3087,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A237" authorId="0">
+    <comment ref="A238" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3087,7 +3100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A238" authorId="0">
+    <comment ref="A239" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3100,7 +3113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A239" authorId="0">
+    <comment ref="A240" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3113,7 +3126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A240" authorId="0">
+    <comment ref="A241" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3126,7 +3139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A241" authorId="0">
+    <comment ref="A242" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3139,7 +3152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A242" authorId="0">
+    <comment ref="A243" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3152,7 +3165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A243" authorId="0">
+    <comment ref="A244" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3165,7 +3178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A244" authorId="0">
+    <comment ref="A245" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3178,7 +3191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A245" authorId="0">
+    <comment ref="A246" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3191,7 +3204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A246" authorId="0">
+    <comment ref="A247" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3204,7 +3217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A247" authorId="0">
+    <comment ref="A248" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3217,7 +3230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A248" authorId="0">
+    <comment ref="A249" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3230,7 +3243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A249" authorId="0">
+    <comment ref="A250" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3243,7 +3256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A250" authorId="0">
+    <comment ref="A251" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3256,7 +3269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A251" authorId="0">
+    <comment ref="A252" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3269,7 +3282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A252" authorId="0">
+    <comment ref="A253" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3282,7 +3295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A253" authorId="0">
+    <comment ref="A254" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3295,7 +3308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A254" authorId="0">
+    <comment ref="A255" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3308,7 +3321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A255" authorId="0">
+    <comment ref="A256" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3321,7 +3334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A256" authorId="0">
+    <comment ref="A257" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3334,7 +3347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A257" authorId="0">
+    <comment ref="A258" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3347,7 +3360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A258" authorId="0">
+    <comment ref="A259" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3360,7 +3373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A259" authorId="0">
+    <comment ref="A260" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3373,7 +3386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A260" authorId="0">
+    <comment ref="A261" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3386,7 +3399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A261" authorId="0">
+    <comment ref="A262" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3399,7 +3412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A262" authorId="0">
+    <comment ref="A263" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3412,7 +3425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A263" authorId="0">
+    <comment ref="A264" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3425,7 +3438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A264" authorId="0">
+    <comment ref="A265" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3438,7 +3451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A265" authorId="0">
+    <comment ref="A266" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3451,7 +3464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A266" authorId="0">
+    <comment ref="A267" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3464,7 +3477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A267" authorId="0">
+    <comment ref="A268" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3477,7 +3490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A268" authorId="0">
+    <comment ref="A269" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3490,7 +3503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A269" authorId="0">
+    <comment ref="A270" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3503,7 +3516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A270" authorId="0">
+    <comment ref="A271" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3516,7 +3529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A271" authorId="0">
+    <comment ref="A272" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3529,7 +3542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A272" authorId="0">
+    <comment ref="A273" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3542,7 +3555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A273" authorId="0">
+    <comment ref="A274" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3555,7 +3568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A274" authorId="0">
+    <comment ref="A275" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3568,7 +3581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A275" authorId="0">
+    <comment ref="A276" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3581,7 +3594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A276" authorId="0">
+    <comment ref="A277" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3594,7 +3607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A277" authorId="0">
+    <comment ref="A278" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3607,7 +3620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A278" authorId="0">
+    <comment ref="A279" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3620,7 +3633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A279" authorId="0">
+    <comment ref="A280" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3633,7 +3646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A280" authorId="0">
+    <comment ref="A281" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3646,7 +3659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A281" authorId="0">
+    <comment ref="A282" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3659,7 +3672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A282" authorId="0">
+    <comment ref="A283" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3672,7 +3685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A283" authorId="0">
+    <comment ref="A284" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3685,7 +3698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A284" authorId="0">
+    <comment ref="A285" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3698,7 +3711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A285" authorId="0">
+    <comment ref="A286" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3711,7 +3724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A286" authorId="0">
+    <comment ref="A287" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3724,7 +3737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A287" authorId="0">
+    <comment ref="A288" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3737,7 +3750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A288" authorId="0">
+    <comment ref="A289" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3750,7 +3763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A289" authorId="0">
+    <comment ref="A290" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3763,7 +3776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A290" authorId="0">
+    <comment ref="A291" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3776,7 +3789,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A291" authorId="0">
+    <comment ref="A292" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3789,7 +3802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A292" authorId="0">
+    <comment ref="A293" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3802,7 +3815,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A293" authorId="0">
+    <comment ref="A294" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3815,7 +3828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A294" authorId="0">
+    <comment ref="A295" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3828,7 +3841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A295" authorId="0">
+    <comment ref="A296" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3841,7 +3854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A296" authorId="0">
+    <comment ref="A297" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3854,7 +3867,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A297" authorId="0">
+    <comment ref="A298" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3867,7 +3880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A298" authorId="0">
+    <comment ref="A299" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3880,7 +3893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A299" authorId="0">
+    <comment ref="A300" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3893,7 +3906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A300" authorId="0">
+    <comment ref="A301" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3906,7 +3919,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A301" authorId="0">
+    <comment ref="A302" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3919,7 +3932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A302" authorId="0">
+    <comment ref="A303" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3932,7 +3945,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A303" authorId="0">
+    <comment ref="A304" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3945,7 +3958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A304" authorId="0">
+    <comment ref="A305" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3958,7 +3971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A305" authorId="0">
+    <comment ref="A306" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3976,7 +3989,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="363">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -4690,6 +4703,9 @@
   </si>
   <si>
     <t>parent_id</t>
+  </si>
+  <si>
+    <t>parent_sample_id</t>
   </si>
   <si>
     <t>pathologist_report</t>
@@ -5402,7 +5418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF305"/>
+  <dimension ref="A1:BF306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -8874,9 +8890,6 @@
       <c r="T181" t="s">
         <v>58</v>
       </c>
-      <c r="U181" t="s">
-        <v>58</v>
-      </c>
       <c r="V181" t="s">
         <v>58</v>
       </c>
@@ -8966,7 +8979,7 @@
       <c r="A182" t="s">
         <v>238</v>
       </c>
-      <c r="AP182" t="s">
+      <c r="U182" t="s">
         <v>58</v>
       </c>
     </row>
@@ -8974,7 +8987,7 @@
       <c r="A183" t="s">
         <v>239</v>
       </c>
-      <c r="AQ183" t="s">
+      <c r="AP183" t="s">
         <v>58</v>
       </c>
     </row>
@@ -8990,7 +9003,7 @@
       <c r="A185" t="s">
         <v>241</v>
       </c>
-      <c r="AK185" t="s">
+      <c r="AQ185" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9001,93 +9014,15 @@
       <c r="AK186" t="s">
         <v>58</v>
       </c>
-      <c r="AP186" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="187" spans="1:58">
       <c r="A187" t="s">
         <v>243</v>
       </c>
-      <c r="C187" t="s">
-        <v>58</v>
-      </c>
-      <c r="E187" t="s">
-        <v>58</v>
-      </c>
-      <c r="F187" t="s">
-        <v>58</v>
-      </c>
-      <c r="G187" t="s">
-        <v>58</v>
-      </c>
-      <c r="H187" t="s">
-        <v>58</v>
-      </c>
-      <c r="I187" t="s">
-        <v>58</v>
-      </c>
-      <c r="J187" t="s">
-        <v>58</v>
-      </c>
-      <c r="R187" t="s">
-        <v>58</v>
-      </c>
-      <c r="V187" t="s">
-        <v>58</v>
-      </c>
-      <c r="W187" t="s">
-        <v>58</v>
-      </c>
-      <c r="X187" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y187" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX187" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ187" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA187" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC187" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE187" t="s">
+      <c r="AK187" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP187" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9181,7 +9116,85 @@
       <c r="A189" t="s">
         <v>245</v>
       </c>
+      <c r="C189" t="s">
+        <v>58</v>
+      </c>
+      <c r="E189" t="s">
+        <v>58</v>
+      </c>
+      <c r="F189" t="s">
+        <v>58</v>
+      </c>
+      <c r="G189" t="s">
+        <v>58</v>
+      </c>
+      <c r="H189" t="s">
+        <v>58</v>
+      </c>
+      <c r="I189" t="s">
+        <v>58</v>
+      </c>
+      <c r="J189" t="s">
+        <v>58</v>
+      </c>
+      <c r="R189" t="s">
+        <v>58</v>
+      </c>
+      <c r="V189" t="s">
+        <v>58</v>
+      </c>
+      <c r="W189" t="s">
+        <v>58</v>
+      </c>
+      <c r="X189" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y189" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z189" t="s">
+        <v>58</v>
+      </c>
       <c r="AD189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX189" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ189" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA189" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC189" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE189" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9229,19 +9242,7 @@
       <c r="A195" t="s">
         <v>251</v>
       </c>
-      <c r="E195" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE195" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF195" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ195" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC195" t="s">
+      <c r="AD195" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9269,19 +9270,19 @@
       <c r="A197" t="s">
         <v>253</v>
       </c>
-      <c r="I197" t="s">
-        <v>58</v>
-      </c>
-      <c r="R197" t="s">
-        <v>58</v>
-      </c>
-      <c r="X197" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y197" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH197" t="s">
+      <c r="E197" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE197" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF197" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ197" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC197" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9289,13 +9290,19 @@
       <c r="A198" t="s">
         <v>254</v>
       </c>
-      <c r="AQ198" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR198" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS198" t="s">
+      <c r="I198" t="s">
+        <v>58</v>
+      </c>
+      <c r="R198" t="s">
+        <v>58</v>
+      </c>
+      <c r="X198" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y198" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH198" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9303,22 +9310,13 @@
       <c r="A199" t="s">
         <v>255</v>
       </c>
-      <c r="J199" t="s">
-        <v>58</v>
-      </c>
-      <c r="V199" t="s">
-        <v>58</v>
-      </c>
-      <c r="W199" t="s">
-        <v>58</v>
-      </c>
-      <c r="X199" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD199" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX199" t="s">
+      <c r="AQ199" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR199" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS199" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9349,7 +9347,22 @@
       <c r="A201" t="s">
         <v>257</v>
       </c>
+      <c r="J201" t="s">
+        <v>58</v>
+      </c>
+      <c r="V201" t="s">
+        <v>58</v>
+      </c>
+      <c r="W201" t="s">
+        <v>58</v>
+      </c>
       <c r="X201" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD201" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX201" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9357,13 +9370,7 @@
       <c r="A202" t="s">
         <v>258</v>
       </c>
-      <c r="AQ202" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR202" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS202" t="s">
+      <c r="X202" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9371,7 +9378,13 @@
       <c r="A203" t="s">
         <v>259</v>
       </c>
-      <c r="X203" t="s">
+      <c r="AQ203" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR203" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS203" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9379,7 +9392,7 @@
       <c r="A204" t="s">
         <v>260</v>
       </c>
-      <c r="AD204" t="s">
+      <c r="X204" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9403,7 +9416,7 @@
       <c r="A207" t="s">
         <v>263</v>
       </c>
-      <c r="BC207" t="s">
+      <c r="AD207" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9411,7 +9424,7 @@
       <c r="A208" t="s">
         <v>264</v>
       </c>
-      <c r="AP208" t="s">
+      <c r="BC208" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9419,19 +9432,7 @@
       <c r="A209" t="s">
         <v>265</v>
       </c>
-      <c r="H209" t="s">
-        <v>58</v>
-      </c>
-      <c r="I209" t="s">
-        <v>58</v>
-      </c>
-      <c r="X209" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y209" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH209" t="s">
+      <c r="AP209" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9439,13 +9440,19 @@
       <c r="A210" t="s">
         <v>266</v>
       </c>
+      <c r="H210" t="s">
+        <v>58</v>
+      </c>
       <c r="I210" t="s">
         <v>58</v>
       </c>
-      <c r="R210" t="s">
+      <c r="X210" t="s">
         <v>58</v>
       </c>
       <c r="Y210" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH210" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9453,13 +9460,13 @@
       <c r="A211" t="s">
         <v>267</v>
       </c>
-      <c r="AQ211" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR211" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS211" t="s">
+      <c r="I211" t="s">
+        <v>58</v>
+      </c>
+      <c r="R211" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y211" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9481,85 +9488,13 @@
       <c r="A213" t="s">
         <v>269</v>
       </c>
-      <c r="C213" t="s">
-        <v>58</v>
-      </c>
-      <c r="E213" t="s">
-        <v>58</v>
-      </c>
-      <c r="F213" t="s">
-        <v>58</v>
-      </c>
-      <c r="G213" t="s">
-        <v>58</v>
-      </c>
-      <c r="H213" t="s">
-        <v>58</v>
-      </c>
-      <c r="I213" t="s">
-        <v>58</v>
-      </c>
-      <c r="J213" t="s">
-        <v>58</v>
-      </c>
-      <c r="R213" t="s">
-        <v>58</v>
-      </c>
-      <c r="V213" t="s">
-        <v>58</v>
-      </c>
-      <c r="W213" t="s">
-        <v>58</v>
-      </c>
-      <c r="X213" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y213" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX213" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ213" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA213" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC213" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE213" t="s">
+      <c r="AQ213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR213" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS213" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9567,7 +9502,85 @@
       <c r="A214" t="s">
         <v>270</v>
       </c>
+      <c r="C214" t="s">
+        <v>58</v>
+      </c>
+      <c r="E214" t="s">
+        <v>58</v>
+      </c>
+      <c r="F214" t="s">
+        <v>58</v>
+      </c>
+      <c r="G214" t="s">
+        <v>58</v>
+      </c>
+      <c r="H214" t="s">
+        <v>58</v>
+      </c>
+      <c r="I214" t="s">
+        <v>58</v>
+      </c>
+      <c r="J214" t="s">
+        <v>58</v>
+      </c>
+      <c r="R214" t="s">
+        <v>58</v>
+      </c>
+      <c r="V214" t="s">
+        <v>58</v>
+      </c>
+      <c r="W214" t="s">
+        <v>58</v>
+      </c>
+      <c r="X214" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y214" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV214" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX214" t="s">
+        <v>58</v>
+      </c>
       <c r="AZ214" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA214" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC214" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE214" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9575,13 +9588,7 @@
       <c r="A215" t="s">
         <v>271</v>
       </c>
-      <c r="AQ215" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR215" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS215" t="s">
+      <c r="AZ215" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9589,7 +9596,13 @@
       <c r="A216" t="s">
         <v>272</v>
       </c>
-      <c r="BC216" t="s">
+      <c r="AQ216" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR216" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS216" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9597,7 +9610,7 @@
       <c r="A217" t="s">
         <v>273</v>
       </c>
-      <c r="Z217" t="s">
+      <c r="BC217" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9613,22 +9626,7 @@
       <c r="A219" t="s">
         <v>275</v>
       </c>
-      <c r="J219" t="s">
-        <v>58</v>
-      </c>
-      <c r="V219" t="s">
-        <v>58</v>
-      </c>
-      <c r="W219" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD219" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG219" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX219" t="s">
+      <c r="Z219" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9636,7 +9634,22 @@
       <c r="A220" t="s">
         <v>276</v>
       </c>
-      <c r="AF220" t="s">
+      <c r="J220" t="s">
+        <v>58</v>
+      </c>
+      <c r="V220" t="s">
+        <v>58</v>
+      </c>
+      <c r="W220" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD220" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG220" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX220" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9644,58 +9657,7 @@
       <c r="A221" t="s">
         <v>277</v>
       </c>
-      <c r="C221" t="s">
-        <v>58</v>
-      </c>
-      <c r="E221" t="s">
-        <v>58</v>
-      </c>
-      <c r="H221" t="s">
-        <v>58</v>
-      </c>
-      <c r="I221" t="s">
-        <v>58</v>
-      </c>
-      <c r="J221" t="s">
-        <v>58</v>
-      </c>
-      <c r="R221" t="s">
-        <v>58</v>
-      </c>
-      <c r="X221" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y221" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z221" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD221" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE221" t="s">
-        <v>58</v>
-      </c>
       <c r="AF221" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG221" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH221" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ221" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX221" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA221" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC221" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9886,16 +9848,40 @@
       <c r="E225" t="s">
         <v>58</v>
       </c>
+      <c r="H225" t="s">
+        <v>58</v>
+      </c>
+      <c r="I225" t="s">
+        <v>58</v>
+      </c>
       <c r="J225" t="s">
         <v>58</v>
       </c>
+      <c r="R225" t="s">
+        <v>58</v>
+      </c>
+      <c r="X225" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y225" t="s">
+        <v>58</v>
+      </c>
       <c r="Z225" t="s">
         <v>58</v>
       </c>
+      <c r="AD225" t="s">
+        <v>58</v>
+      </c>
       <c r="AE225" t="s">
         <v>58</v>
       </c>
       <c r="AF225" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG225" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH225" t="s">
         <v>58</v>
       </c>
       <c r="AJ225" t="s">
@@ -9950,10 +9936,34 @@
       <c r="A227" t="s">
         <v>283</v>
       </c>
-      <c r="AU227" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV227" t="s">
+      <c r="C227" t="s">
+        <v>58</v>
+      </c>
+      <c r="E227" t="s">
+        <v>58</v>
+      </c>
+      <c r="J227" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z227" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE227" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF227" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ227" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX227" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA227" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC227" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9961,7 +9971,10 @@
       <c r="A228" t="s">
         <v>284</v>
       </c>
-      <c r="G228" t="s">
+      <c r="AU228" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV228" t="s">
         <v>58</v>
       </c>
     </row>
@@ -9980,42 +9993,21 @@
       <c r="G230" t="s">
         <v>58</v>
       </c>
-      <c r="AU230" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV230" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ230" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="231" spans="1:55">
       <c r="A231" t="s">
         <v>287</v>
       </c>
-      <c r="E231" t="s">
-        <v>58</v>
-      </c>
-      <c r="V231" t="s">
-        <v>58</v>
-      </c>
-      <c r="W231" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD231" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE231" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF231" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ231" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC231" t="s">
+      <c r="G231" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU231" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV231" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ231" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10052,7 +10044,28 @@
       <c r="A233" t="s">
         <v>289</v>
       </c>
-      <c r="D233" t="s">
+      <c r="E233" t="s">
+        <v>58</v>
+      </c>
+      <c r="V233" t="s">
+        <v>58</v>
+      </c>
+      <c r="W233" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD233" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE233" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF233" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ233" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC233" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10060,16 +10073,7 @@
       <c r="A234" t="s">
         <v>290</v>
       </c>
-      <c r="AP234" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ234" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR234" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS234" t="s">
+      <c r="D234" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10077,7 +10081,16 @@
       <c r="A235" t="s">
         <v>291</v>
       </c>
-      <c r="F235" t="s">
+      <c r="AP235" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ235" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR235" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS235" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10085,13 +10098,7 @@
       <c r="A236" t="s">
         <v>292</v>
       </c>
-      <c r="AT236" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU236" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV236" t="s">
+      <c r="F236" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10169,7 +10176,13 @@
       <c r="A242" t="s">
         <v>298</v>
       </c>
-      <c r="AF242" t="s">
+      <c r="AT242" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU242" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV242" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10177,7 +10190,7 @@
       <c r="A243" t="s">
         <v>299</v>
       </c>
-      <c r="AR243" t="s">
+      <c r="AF243" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10185,37 +10198,7 @@
       <c r="A244" t="s">
         <v>300</v>
       </c>
-      <c r="I244" t="s">
-        <v>58</v>
-      </c>
-      <c r="J244" t="s">
-        <v>58</v>
-      </c>
-      <c r="R244" t="s">
-        <v>58</v>
-      </c>
-      <c r="V244" t="s">
-        <v>58</v>
-      </c>
-      <c r="W244" t="s">
-        <v>58</v>
-      </c>
-      <c r="X244" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y244" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD244" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG244" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX244" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA244" t="s">
+      <c r="AR244" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10223,7 +10206,37 @@
       <c r="A245" t="s">
         <v>301</v>
       </c>
-      <c r="AR245" t="s">
+      <c r="I245" t="s">
+        <v>58</v>
+      </c>
+      <c r="J245" t="s">
+        <v>58</v>
+      </c>
+      <c r="R245" t="s">
+        <v>58</v>
+      </c>
+      <c r="V245" t="s">
+        <v>58</v>
+      </c>
+      <c r="W245" t="s">
+        <v>58</v>
+      </c>
+      <c r="X245" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y245" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD245" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG245" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX245" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA245" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10239,13 +10252,7 @@
       <c r="A247" t="s">
         <v>303</v>
       </c>
-      <c r="V247" t="s">
-        <v>58</v>
-      </c>
-      <c r="W247" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD247" t="s">
+      <c r="AR247" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10253,7 +10260,13 @@
       <c r="A248" t="s">
         <v>304</v>
       </c>
-      <c r="AF248" t="s">
+      <c r="V248" t="s">
+        <v>58</v>
+      </c>
+      <c r="W248" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD248" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10261,25 +10274,7 @@
       <c r="A249" t="s">
         <v>305</v>
       </c>
-      <c r="F249" t="s">
-        <v>58</v>
-      </c>
-      <c r="G249" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT249" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU249" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV249" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ249" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE249" t="s">
+      <c r="AF249" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10365,13 +10360,25 @@
       <c r="A253" t="s">
         <v>309</v>
       </c>
-      <c r="V253" t="s">
-        <v>58</v>
-      </c>
-      <c r="W253" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD253" t="s">
+      <c r="F253" t="s">
+        <v>58</v>
+      </c>
+      <c r="G253" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT253" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU253" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV253" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ253" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE253" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10379,19 +10386,13 @@
       <c r="A254" t="s">
         <v>310</v>
       </c>
-      <c r="E254" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE254" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF254" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ254" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC254" t="s">
+      <c r="V254" t="s">
+        <v>58</v>
+      </c>
+      <c r="W254" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD254" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10399,7 +10400,19 @@
       <c r="A255" t="s">
         <v>311</v>
       </c>
+      <c r="E255" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE255" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF255" t="s">
+        <v>58</v>
+      </c>
       <c r="AJ255" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC255" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10415,7 +10428,7 @@
       <c r="A257" t="s">
         <v>313</v>
       </c>
-      <c r="AV257" t="s">
+      <c r="AJ257" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10423,13 +10436,7 @@
       <c r="A258" t="s">
         <v>314</v>
       </c>
-      <c r="AQ258" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR258" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS258" t="s">
+      <c r="AV258" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10451,13 +10458,13 @@
       <c r="A260" t="s">
         <v>316</v>
       </c>
-      <c r="I260" t="s">
-        <v>58</v>
-      </c>
-      <c r="R260" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y260" t="s">
+      <c r="AQ260" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR260" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS260" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10493,7 +10500,13 @@
       <c r="A263" t="s">
         <v>319</v>
       </c>
-      <c r="AP263" t="s">
+      <c r="I263" t="s">
+        <v>58</v>
+      </c>
+      <c r="R263" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y263" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10525,7 +10538,7 @@
       <c r="A267" t="s">
         <v>323</v>
       </c>
-      <c r="BC267" t="s">
+      <c r="AP267" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10533,7 +10546,7 @@
       <c r="A268" t="s">
         <v>324</v>
       </c>
-      <c r="BA268" t="s">
+      <c r="BC268" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10541,10 +10554,7 @@
       <c r="A269" t="s">
         <v>325</v>
       </c>
-      <c r="V269" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD269" t="s">
+      <c r="BA269" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10552,7 +10562,10 @@
       <c r="A270" t="s">
         <v>326</v>
       </c>
-      <c r="Z270" t="s">
+      <c r="V270" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD270" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10560,13 +10573,7 @@
       <c r="A271" t="s">
         <v>327</v>
       </c>
-      <c r="AQ271" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR271" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS271" t="s">
+      <c r="Z271" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10588,6 +10595,12 @@
       <c r="A273" t="s">
         <v>329</v>
       </c>
+      <c r="AQ273" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR273" t="s">
+        <v>58</v>
+      </c>
       <c r="AS273" t="s">
         <v>58</v>
       </c>
@@ -10620,85 +10633,7 @@
       <c r="A277" t="s">
         <v>333</v>
       </c>
-      <c r="C277" t="s">
-        <v>58</v>
-      </c>
-      <c r="E277" t="s">
-        <v>58</v>
-      </c>
-      <c r="F277" t="s">
-        <v>58</v>
-      </c>
-      <c r="G277" t="s">
-        <v>58</v>
-      </c>
-      <c r="H277" t="s">
-        <v>58</v>
-      </c>
-      <c r="I277" t="s">
-        <v>58</v>
-      </c>
-      <c r="J277" t="s">
-        <v>58</v>
-      </c>
-      <c r="R277" t="s">
-        <v>58</v>
-      </c>
-      <c r="V277" t="s">
-        <v>58</v>
-      </c>
-      <c r="W277" t="s">
-        <v>58</v>
-      </c>
-      <c r="X277" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y277" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX277" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ277" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA277" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC277" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE277" t="s">
+      <c r="AS277" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10706,7 +10641,85 @@
       <c r="A278" t="s">
         <v>334</v>
       </c>
-      <c r="AK278" t="s">
+      <c r="C278" t="s">
+        <v>58</v>
+      </c>
+      <c r="E278" t="s">
+        <v>58</v>
+      </c>
+      <c r="F278" t="s">
+        <v>58</v>
+      </c>
+      <c r="G278" t="s">
+        <v>58</v>
+      </c>
+      <c r="H278" t="s">
+        <v>58</v>
+      </c>
+      <c r="I278" t="s">
+        <v>58</v>
+      </c>
+      <c r="J278" t="s">
+        <v>58</v>
+      </c>
+      <c r="R278" t="s">
+        <v>58</v>
+      </c>
+      <c r="V278" t="s">
+        <v>58</v>
+      </c>
+      <c r="W278" t="s">
+        <v>58</v>
+      </c>
+      <c r="X278" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y278" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX278" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ278" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA278" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC278" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE278" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10722,10 +10735,7 @@
       <c r="A280" t="s">
         <v>336</v>
       </c>
-      <c r="AE280" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ280" t="s">
+      <c r="AK280" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10733,7 +10743,10 @@
       <c r="A281" t="s">
         <v>337</v>
       </c>
-      <c r="AK281" t="s">
+      <c r="AE281" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ281" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10741,7 +10754,7 @@
       <c r="A282" t="s">
         <v>338</v>
       </c>
-      <c r="AT282" t="s">
+      <c r="AK282" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10749,9 +10762,6 @@
       <c r="A283" t="s">
         <v>339</v>
       </c>
-      <c r="F283" t="s">
-        <v>58</v>
-      </c>
       <c r="AT283" t="s">
         <v>58</v>
       </c>
@@ -10782,13 +10792,10 @@
       <c r="A286" t="s">
         <v>342</v>
       </c>
-      <c r="AQ286" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR286" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS286" t="s">
+      <c r="F286" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT286" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10796,7 +10803,13 @@
       <c r="A287" t="s">
         <v>343</v>
       </c>
-      <c r="AU287" t="s">
+      <c r="AQ287" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR287" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS287" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10820,7 +10833,7 @@
       <c r="A290" t="s">
         <v>346</v>
       </c>
-      <c r="D290" t="s">
+      <c r="AU290" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10828,100 +10841,7 @@
       <c r="A291" t="s">
         <v>347</v>
       </c>
-      <c r="C291" t="s">
-        <v>58</v>
-      </c>
       <c r="D291" t="s">
-        <v>58</v>
-      </c>
-      <c r="E291" t="s">
-        <v>58</v>
-      </c>
-      <c r="F291" t="s">
-        <v>58</v>
-      </c>
-      <c r="G291" t="s">
-        <v>58</v>
-      </c>
-      <c r="H291" t="s">
-        <v>58</v>
-      </c>
-      <c r="I291" t="s">
-        <v>58</v>
-      </c>
-      <c r="J291" t="s">
-        <v>58</v>
-      </c>
-      <c r="L291" t="s">
-        <v>58</v>
-      </c>
-      <c r="R291" t="s">
-        <v>58</v>
-      </c>
-      <c r="V291" t="s">
-        <v>58</v>
-      </c>
-      <c r="W291" t="s">
-        <v>58</v>
-      </c>
-      <c r="X291" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y291" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX291" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ291" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA291" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC291" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE291" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10929,7 +10849,100 @@
       <c r="A292" t="s">
         <v>348</v>
       </c>
-      <c r="AP292" t="s">
+      <c r="C292" t="s">
+        <v>58</v>
+      </c>
+      <c r="D292" t="s">
+        <v>58</v>
+      </c>
+      <c r="E292" t="s">
+        <v>58</v>
+      </c>
+      <c r="F292" t="s">
+        <v>58</v>
+      </c>
+      <c r="G292" t="s">
+        <v>58</v>
+      </c>
+      <c r="H292" t="s">
+        <v>58</v>
+      </c>
+      <c r="I292" t="s">
+        <v>58</v>
+      </c>
+      <c r="J292" t="s">
+        <v>58</v>
+      </c>
+      <c r="L292" t="s">
+        <v>58</v>
+      </c>
+      <c r="R292" t="s">
+        <v>58</v>
+      </c>
+      <c r="V292" t="s">
+        <v>58</v>
+      </c>
+      <c r="W292" t="s">
+        <v>58</v>
+      </c>
+      <c r="X292" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y292" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX292" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ292" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA292" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC292" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE292" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10937,7 +10950,7 @@
       <c r="A293" t="s">
         <v>349</v>
       </c>
-      <c r="AE293" t="s">
+      <c r="AP293" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10953,7 +10966,7 @@
       <c r="A295" t="s">
         <v>351</v>
       </c>
-      <c r="AJ295" t="s">
+      <c r="AE295" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10961,7 +10974,7 @@
       <c r="A296" t="s">
         <v>352</v>
       </c>
-      <c r="AQ296" t="s">
+      <c r="AJ296" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10977,7 +10990,7 @@
       <c r="A298" t="s">
         <v>354</v>
       </c>
-      <c r="AP298" t="s">
+      <c r="AQ298" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10993,7 +11006,7 @@
       <c r="A300" t="s">
         <v>356</v>
       </c>
-      <c r="AK300" t="s">
+      <c r="AP300" t="s">
         <v>58</v>
       </c>
     </row>
@@ -11009,7 +11022,7 @@
       <c r="A302" t="s">
         <v>358</v>
       </c>
-      <c r="AJ302" t="s">
+      <c r="AK302" t="s">
         <v>58</v>
       </c>
     </row>
@@ -11025,10 +11038,7 @@
       <c r="A304" t="s">
         <v>360</v>
       </c>
-      <c r="AK304" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ304" t="s">
+      <c r="AJ304" t="s">
         <v>58</v>
       </c>
     </row>
@@ -11036,7 +11046,18 @@
       <c r="A305" t="s">
         <v>361</v>
       </c>
+      <c r="AK305" t="s">
+        <v>58</v>
+      </c>
       <c r="AQ305" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="306" spans="1:43">
+      <c r="A306" t="s">
+        <v>362</v>
+      </c>
+      <c r="AQ306" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Metadata Release] New release per 11/09/2023 #1246  (#1249)
* update antibodies metadata to v3
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3989,7 +3989,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="363">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -7418,6 +7418,9 @@
       <c r="C99" t="s">
         <v>58</v>
       </c>
+      <c r="D99" t="s">
+        <v>58</v>
+      </c>
       <c r="E99" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Nihdev 427 ivt assay removals (#1254)
* Docs: Removals

* Docs: Test fixes

* Docs: Add some text to explain the current/deprecated split

* Docs: Add nanoSPLITS back

* Docs: Add nanoSPLITS back

* Docs: Update field-schemas

---------

Co-authored-by: Juan Puerto <=>
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -3989,7 +3989,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="364">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -4096,6 +4096,9 @@
     <t>nano</t>
   </si>
   <si>
+    <t>nano-splits</t>
+  </si>
+  <si>
     <t>oct</t>
   </si>
   <si>
@@ -4109,9 +4112,6 @@
   </si>
   <si>
     <t>rnaseq</t>
-  </si>
-  <si>
-    <t>rnaseq-geomx</t>
   </si>
   <si>
     <t>sample</t>
@@ -5750,7 +5750,7 @@
       <c r="AJ9" t="s">
         <v>59</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>59</v>
       </c>
       <c r="AU9" t="s">
@@ -5836,7 +5836,7 @@
       <c r="AJ10" t="s">
         <v>59</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
         <v>59</v>
       </c>
       <c r="AU10" t="s">
@@ -6137,7 +6137,7 @@
       <c r="AM21" t="s">
         <v>59</v>
       </c>
-      <c r="AO21" t="s">
+      <c r="AN21" t="s">
         <v>59</v>
       </c>
       <c r="AP21" t="s">
@@ -6566,7 +6566,7 @@
       <c r="A45" t="s">
         <v>102</v>
       </c>
-      <c r="AL45" t="s">
+      <c r="AM45" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6574,7 +6574,7 @@
       <c r="A46" t="s">
         <v>103</v>
       </c>
-      <c r="AL46" t="s">
+      <c r="AM46" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6724,10 +6724,10 @@
       <c r="AJ58" t="s">
         <v>59</v>
       </c>
-      <c r="AK58" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN58" t="s">
+      <c r="AL58" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO58" t="s">
         <v>59</v>
       </c>
       <c r="AU58" t="s">
@@ -6843,10 +6843,10 @@
       <c r="AJ62" t="s">
         <v>59</v>
       </c>
-      <c r="AK62" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN62" t="s">
+      <c r="AL62" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO62" t="s">
         <v>59</v>
       </c>
       <c r="AU62" t="s">
@@ -6943,7 +6943,7 @@
       <c r="AJ64" t="s">
         <v>59</v>
       </c>
-      <c r="AK64" t="s">
+      <c r="AL64" t="s">
         <v>59</v>
       </c>
       <c r="AU64" t="s">
@@ -7082,7 +7082,7 @@
       <c r="AJ72" t="s">
         <v>59</v>
       </c>
-      <c r="AK72" t="s">
+      <c r="AL72" t="s">
         <v>59</v>
       </c>
       <c r="AU72" t="s">
@@ -7214,7 +7214,7 @@
       <c r="AJ78" t="s">
         <v>59</v>
       </c>
-      <c r="AK78" t="s">
+      <c r="AL78" t="s">
         <v>59</v>
       </c>
       <c r="AU78" t="s">
@@ -7442,9 +7442,6 @@
       <c r="I99" t="s">
         <v>59</v>
       </c>
-      <c r="J99" t="s">
-        <v>59</v>
-      </c>
       <c r="K99" t="s">
         <v>59</v>
       </c>
@@ -7469,9 +7466,6 @@
       <c r="R99" t="s">
         <v>59</v>
       </c>
-      <c r="S99" t="s">
-        <v>59</v>
-      </c>
       <c r="T99" t="s">
         <v>59</v>
       </c>
@@ -7569,9 +7563,6 @@
         <v>59</v>
       </c>
       <c r="BE99" t="s">
-        <v>59</v>
-      </c>
-      <c r="BF99" t="s">
         <v>59</v>
       </c>
       <c r="BG99" t="s">
@@ -7681,7 +7672,7 @@
       <c r="A103" t="s">
         <v>160</v>
       </c>
-      <c r="AL103" t="s">
+      <c r="AM103" t="s">
         <v>59</v>
       </c>
     </row>
@@ -7719,7 +7710,7 @@
       <c r="A107" t="s">
         <v>164</v>
       </c>
-      <c r="AL107" t="s">
+      <c r="AM107" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8156,7 +8147,7 @@
       <c r="AH141" t="s">
         <v>59</v>
       </c>
-      <c r="AK141" t="s">
+      <c r="AL141" t="s">
         <v>59</v>
       </c>
       <c r="BD141" t="s">
@@ -8185,7 +8176,7 @@
       <c r="AH142" t="s">
         <v>59</v>
       </c>
-      <c r="AK142" t="s">
+      <c r="AL142" t="s">
         <v>59</v>
       </c>
       <c r="BD142" t="s">
@@ -8214,7 +8205,7 @@
       <c r="AH143" t="s">
         <v>59</v>
       </c>
-      <c r="AK143" t="s">
+      <c r="AL143" t="s">
         <v>59</v>
       </c>
       <c r="BD143" t="s">
@@ -8243,7 +8234,7 @@
       <c r="AH144" t="s">
         <v>59</v>
       </c>
-      <c r="AK144" t="s">
+      <c r="AL144" t="s">
         <v>59</v>
       </c>
       <c r="BD144" t="s">
@@ -8493,7 +8484,7 @@
       <c r="AH161" t="s">
         <v>59</v>
       </c>
-      <c r="AK161" t="s">
+      <c r="AL161" t="s">
         <v>59</v>
       </c>
       <c r="BD161" t="s">
@@ -8590,7 +8581,7 @@
       <c r="AJ166" t="s">
         <v>59</v>
       </c>
-      <c r="AK166" t="s">
+      <c r="AL166" t="s">
         <v>59</v>
       </c>
       <c r="AU166" t="s">
@@ -8676,7 +8667,7 @@
       <c r="AJ167" t="s">
         <v>59</v>
       </c>
-      <c r="AK167" t="s">
+      <c r="AL167" t="s">
         <v>59</v>
       </c>
       <c r="AU167" t="s">
@@ -8716,7 +8707,7 @@
       <c r="A169" t="s">
         <v>226</v>
       </c>
-      <c r="AL169" t="s">
+      <c r="AM169" t="s">
         <v>59</v>
       </c>
       <c r="AQ169" t="s">
@@ -8727,7 +8718,7 @@
       <c r="A170" t="s">
         <v>227</v>
       </c>
-      <c r="AL170" t="s">
+      <c r="AM170" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8735,7 +8726,7 @@
       <c r="A171" t="s">
         <v>228</v>
       </c>
-      <c r="AL171" t="s">
+      <c r="AM171" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8743,7 +8734,7 @@
       <c r="A172" t="s">
         <v>229</v>
       </c>
-      <c r="AL172" t="s">
+      <c r="AM172" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8751,7 +8742,7 @@
       <c r="A173" t="s">
         <v>230</v>
       </c>
-      <c r="AL173" t="s">
+      <c r="AM173" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8759,7 +8750,7 @@
       <c r="A174" t="s">
         <v>231</v>
       </c>
-      <c r="AL174" t="s">
+      <c r="AM174" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8767,7 +8758,7 @@
       <c r="A175" t="s">
         <v>232</v>
       </c>
-      <c r="AL175" t="s">
+      <c r="AM175" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8775,7 +8766,7 @@
       <c r="A176" t="s">
         <v>233</v>
       </c>
-      <c r="AL176" t="s">
+      <c r="AM176" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8783,7 +8774,7 @@
       <c r="A177" t="s">
         <v>234</v>
       </c>
-      <c r="AL177" t="s">
+      <c r="AM177" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8791,7 +8782,7 @@
       <c r="A178" t="s">
         <v>235</v>
       </c>
-      <c r="AL178" t="s">
+      <c r="AM178" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8799,7 +8790,7 @@
       <c r="A179" t="s">
         <v>236</v>
       </c>
-      <c r="AL179" t="s">
+      <c r="AM179" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8854,9 +8845,6 @@
       <c r="I181" t="s">
         <v>59</v>
       </c>
-      <c r="J181" t="s">
-        <v>59</v>
-      </c>
       <c r="K181" t="s">
         <v>59</v>
       </c>
@@ -8878,9 +8866,6 @@
       <c r="R181" t="s">
         <v>59</v>
       </c>
-      <c r="S181" t="s">
-        <v>59</v>
-      </c>
       <c r="T181" t="s">
         <v>59</v>
       </c>
@@ -8917,10 +8902,7 @@
       <c r="AI181" t="s">
         <v>59</v>
       </c>
-      <c r="AK181" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM181" t="s">
+      <c r="AL181" t="s">
         <v>59</v>
       </c>
       <c r="AN181" t="s">
@@ -8951,9 +8933,6 @@
         <v>59</v>
       </c>
       <c r="BE181" t="s">
-        <v>59</v>
-      </c>
-      <c r="BF181" t="s">
         <v>59</v>
       </c>
       <c r="BG181" t="s">
@@ -8996,7 +8975,7 @@
       <c r="A186" t="s">
         <v>243</v>
       </c>
-      <c r="AL186" t="s">
+      <c r="AM186" t="s">
         <v>59</v>
       </c>
     </row>
@@ -9004,7 +8983,7 @@
       <c r="A187" t="s">
         <v>244</v>
       </c>
-      <c r="AL187" t="s">
+      <c r="AM187" t="s">
         <v>59</v>
       </c>
       <c r="AQ187" t="s">
@@ -9069,7 +9048,7 @@
       <c r="AJ188" t="s">
         <v>59</v>
       </c>
-      <c r="AK188" t="s">
+      <c r="AL188" t="s">
         <v>59</v>
       </c>
       <c r="AU188" t="s">
@@ -9155,7 +9134,7 @@
       <c r="AJ189" t="s">
         <v>59</v>
       </c>
-      <c r="AK189" t="s">
+      <c r="AL189" t="s">
         <v>59</v>
       </c>
       <c r="AU189" t="s">
@@ -9244,7 +9223,7 @@
       <c r="AH196" t="s">
         <v>59</v>
       </c>
-      <c r="AK196" t="s">
+      <c r="AL196" t="s">
         <v>59</v>
       </c>
       <c r="BD196" t="s">
@@ -9264,7 +9243,7 @@
       <c r="AH197" t="s">
         <v>59</v>
       </c>
-      <c r="AK197" t="s">
+      <c r="AL197" t="s">
         <v>59</v>
       </c>
       <c r="BD197" t="s">
@@ -9541,7 +9520,7 @@
       <c r="AJ214" t="s">
         <v>59</v>
       </c>
-      <c r="AK214" t="s">
+      <c r="AL214" t="s">
         <v>59</v>
       </c>
       <c r="AU214" t="s">
@@ -9692,7 +9671,7 @@
       <c r="AJ222" t="s">
         <v>59</v>
       </c>
-      <c r="AK222" t="s">
+      <c r="AL222" t="s">
         <v>59</v>
       </c>
       <c r="AY222" t="s">
@@ -9751,7 +9730,7 @@
       <c r="AJ223" t="s">
         <v>59</v>
       </c>
-      <c r="AK223" t="s">
+      <c r="AL223" t="s">
         <v>59</v>
       </c>
       <c r="AY223" t="s">
@@ -9810,7 +9789,7 @@
       <c r="AJ224" t="s">
         <v>59</v>
       </c>
-      <c r="AK224" t="s">
+      <c r="AL224" t="s">
         <v>59</v>
       </c>
       <c r="AY224" t="s">
@@ -9869,7 +9848,7 @@
       <c r="AJ225" t="s">
         <v>59</v>
       </c>
-      <c r="AK225" t="s">
+      <c r="AL225" t="s">
         <v>59</v>
       </c>
       <c r="AY225" t="s">
@@ -9904,7 +9883,7 @@
       <c r="AH226" t="s">
         <v>59</v>
       </c>
-      <c r="AK226" t="s">
+      <c r="AL226" t="s">
         <v>59</v>
       </c>
       <c r="AY226" t="s">
@@ -9939,7 +9918,7 @@
       <c r="AH227" t="s">
         <v>59</v>
       </c>
-      <c r="AK227" t="s">
+      <c r="AL227" t="s">
         <v>59</v>
       </c>
       <c r="AY227" t="s">
@@ -10018,7 +9997,7 @@
       <c r="AH232" t="s">
         <v>59</v>
       </c>
-      <c r="AK232" t="s">
+      <c r="AL232" t="s">
         <v>59</v>
       </c>
       <c r="BD232" t="s">
@@ -10047,7 +10026,7 @@
       <c r="AH233" t="s">
         <v>59</v>
       </c>
-      <c r="AK233" t="s">
+      <c r="AL233" t="s">
         <v>59</v>
       </c>
       <c r="BD233" t="s">
@@ -10394,7 +10373,7 @@
       <c r="AH255" t="s">
         <v>59</v>
       </c>
-      <c r="AK255" t="s">
+      <c r="AL255" t="s">
         <v>59</v>
       </c>
       <c r="BD255" t="s">
@@ -10405,7 +10384,7 @@
       <c r="A256" t="s">
         <v>313</v>
       </c>
-      <c r="AK256" t="s">
+      <c r="AL256" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10413,7 +10392,7 @@
       <c r="A257" t="s">
         <v>314</v>
       </c>
-      <c r="AK257" t="s">
+      <c r="AL257" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10680,7 +10659,7 @@
       <c r="AJ278" t="s">
         <v>59</v>
       </c>
-      <c r="AK278" t="s">
+      <c r="AL278" t="s">
         <v>59</v>
       </c>
       <c r="AU278" t="s">
@@ -10712,7 +10691,7 @@
       <c r="A279" t="s">
         <v>336</v>
       </c>
-      <c r="AL279" t="s">
+      <c r="AM279" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10720,7 +10699,7 @@
       <c r="A280" t="s">
         <v>337</v>
       </c>
-      <c r="AL280" t="s">
+      <c r="AM280" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10731,7 +10710,7 @@
       <c r="AG281" t="s">
         <v>59</v>
       </c>
-      <c r="AK281" t="s">
+      <c r="AL281" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10739,7 +10718,7 @@
       <c r="A282" t="s">
         <v>339</v>
       </c>
-      <c r="AL282" t="s">
+      <c r="AM282" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10894,10 +10873,10 @@
       <c r="AJ292" t="s">
         <v>59</v>
       </c>
-      <c r="AK292" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN292" t="s">
+      <c r="AL292" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO292" t="s">
         <v>59</v>
       </c>
       <c r="AR292" t="s">
@@ -10959,7 +10938,7 @@
       <c r="A296" t="s">
         <v>353</v>
       </c>
-      <c r="AK296" t="s">
+      <c r="AL296" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10999,7 +10978,7 @@
       <c r="A301" t="s">
         <v>358</v>
       </c>
-      <c r="AL301" t="s">
+      <c r="AM301" t="s">
         <v>59</v>
       </c>
     </row>
@@ -11007,7 +10986,7 @@
       <c r="A302" t="s">
         <v>359</v>
       </c>
-      <c r="AL302" t="s">
+      <c r="AM302" t="s">
         <v>59</v>
       </c>
     </row>
@@ -11015,7 +10994,7 @@
       <c r="A303" t="s">
         <v>360</v>
       </c>
-      <c r="AK303" t="s">
+      <c r="AL303" t="s">
         <v>59</v>
       </c>
     </row>
@@ -11023,7 +11002,7 @@
       <c r="A304" t="s">
         <v>361</v>
       </c>
-      <c r="AK304" t="s">
+      <c r="AL304" t="s">
         <v>59</v>
       </c>
     </row>
@@ -11031,7 +11010,7 @@
       <c r="A305" t="s">
         <v>362</v>
       </c>
-      <c r="AL305" t="s">
+      <c r="AM305" t="s">
         <v>59</v>
       </c>
       <c r="AR305" t="s">

</xml_diff>

<commit_message>
General: Remove CEDAR organ page
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2238,7 +2238,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>UUID or HuBMAP ID of organ</t>
+          <t>Unique HuBMAP identifier for the organ. This can be found in the Submission ID section of a registered donor on the Ingest UI.</t>
         </r>
       </text>
     </comment>
@@ -3989,7 +3989,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="368">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -6164,9 +6164,6 @@
       <c r="AN21" t="s">
         <v>63</v>
       </c>
-      <c r="AO21" t="s">
-        <v>63</v>
-      </c>
       <c r="AP21" t="s">
         <v>63</v>
       </c>
@@ -6346,9 +6343,6 @@
       <c r="AN22" t="s">
         <v>63</v>
       </c>
-      <c r="AO22" t="s">
-        <v>63</v>
-      </c>
       <c r="AP22" t="s">
         <v>63</v>
       </c>
@@ -7566,9 +7560,6 @@
         <v>63</v>
       </c>
       <c r="AN99" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO99" t="s">
         <v>63</v>
       </c>
       <c r="AP99" t="s">

</xml_diff>

<commit_message>
Jpuerto/remove cedar organ (#1271)
* General: Remove CEDAR organ page

* General: Remove CEDAR organ page

---------

Co-authored-by: Juan Puerto <=>
</commit_message>
<xml_diff>
--- a/docs/field-schemas.xlsx
+++ b/docs/field-schemas.xlsx
@@ -2238,7 +2238,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>UUID or HuBMAP ID of organ</t>
+          <t>Unique HuBMAP identifier for the organ. This can be found in the Submission ID section of a registered donor on the Ingest UI.</t>
         </r>
       </text>
     </comment>
@@ -3989,7 +3989,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="368">
   <si>
     <t>10x-multiome</t>
   </si>
@@ -6164,9 +6164,6 @@
       <c r="AN21" t="s">
         <v>63</v>
       </c>
-      <c r="AO21" t="s">
-        <v>63</v>
-      </c>
       <c r="AP21" t="s">
         <v>63</v>
       </c>
@@ -6346,9 +6343,6 @@
       <c r="AN22" t="s">
         <v>63</v>
       </c>
-      <c r="AO22" t="s">
-        <v>63</v>
-      </c>
       <c r="AP22" t="s">
         <v>63</v>
       </c>
@@ -7566,9 +7560,6 @@
         <v>63</v>
       </c>
       <c r="AN99" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO99" t="s">
         <v>63</v>
       </c>
       <c r="AP99" t="s">

</xml_diff>